<commit_message>
Added in proper filtering of the matrix
</commit_message>
<xml_diff>
--- a/master_c4g_24.xlsx
+++ b/master_c4g_24.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakefarren-price/Google Drive/RYA - Analysis/Crew4Gold_24/c4g/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DCEB601-E2CA-364F-BEB6-7327FDBB6758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4F5A7E-E934-DF4D-B348-F8DB0A88BCBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21020" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{1BFC6774-FC3C-7F41-9822-A1F8BB71180D}"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +159,12 @@
   </si>
   <si>
     <t>Will to stretch and challenge themselves</t>
+  </si>
+  <si>
+    <t>Lever</t>
+  </si>
+  <si>
+    <t>Moment</t>
   </si>
 </sst>
 </file>
@@ -226,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -241,10 +247,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -581,21 +590,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63A712AE-29D8-B14A-9818-F49A7E8BD933}">
-  <dimension ref="A1:AA14"/>
+  <dimension ref="A1:AC14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="O15" sqref="O15"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="27" width="15" style="5" customWidth="1"/>
+    <col min="3" max="29" width="15" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="1" customFormat="1" ht="87" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -632,57 +641,66 @@
       <c r="L1" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AB1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AA1" s="6"/>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AC1" s="6"/>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
       </c>
+      <c r="D2" s="5">
+        <v>65</v>
+      </c>
       <c r="E2" s="5">
         <v>180</v>
       </c>
@@ -699,57 +717,68 @@
         <v>356</v>
       </c>
       <c r="M2" s="5">
+        <f>0.58*E2</f>
+        <v>104.39999999999999</v>
+      </c>
+      <c r="N2" s="5">
+        <f>M2*D2</f>
+        <v>6785.9999999999991</v>
+      </c>
+      <c r="O2" s="5">
         <v>1</v>
       </c>
-      <c r="N2" s="5">
+      <c r="P2" s="5">
         <v>2</v>
       </c>
-      <c r="O2" s="5">
-        <v>3</v>
-      </c>
-      <c r="P2" s="5">
-        <v>4</v>
-      </c>
       <c r="Q2" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R2" s="5">
         <v>4</v>
       </c>
       <c r="S2" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T2" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U2" s="5">
         <v>3</v>
       </c>
       <c r="V2" s="5">
+        <v>3</v>
+      </c>
+      <c r="W2" s="5">
+        <v>3</v>
+      </c>
+      <c r="X2" s="5">
         <v>4</v>
       </c>
-      <c r="W2" s="5">
-        <v>5</v>
-      </c>
-      <c r="X2" s="5">
-        <v>5</v>
-      </c>
       <c r="Y2" s="5">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z2" s="5">
+        <v>5</v>
+      </c>
+      <c r="AA2" s="5">
+        <v>3</v>
+      </c>
+      <c r="AB2" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
+      <c r="D3" s="5">
+        <v>70</v>
+      </c>
       <c r="E3" s="5">
-        <v>190</v>
+        <v>165</v>
       </c>
       <c r="F3" s="5">
         <v>2</v>
@@ -764,44 +793,55 @@
         <v>3</v>
       </c>
       <c r="M3" s="5">
-        <f>M2+1</f>
+        <f t="shared" ref="M3:M14" si="0">0.58*E3</f>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="N3" s="5">
+        <f t="shared" ref="N3:N14" si="1">M3*D3</f>
+        <v>6698.9999999999991</v>
+      </c>
+      <c r="O3" s="5">
+        <f>O2+1</f>
         <v>2</v>
       </c>
-      <c r="N3" s="5">
-        <f t="shared" ref="N3:T3" si="0">N2+1</f>
-        <v>3</v>
-      </c>
-      <c r="O3" s="5">
-        <f t="shared" si="0"/>
+      <c r="P3" s="5">
+        <f t="shared" ref="P3:V3" si="2">P2+1</f>
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="P3" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="Q3" s="5">
+      <c r="R3" s="5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="S3" s="5">
         <v>2</v>
       </c>
-      <c r="R3" s="5">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="S3" s="5">
-        <f t="shared" si="0"/>
+      <c r="T3" s="5">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="U3" s="5">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="T3" s="5">
-        <f t="shared" si="0"/>
+      <c r="V3" s="5">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
+      <c r="D4" s="5">
+        <v>60</v>
+      </c>
       <c r="E4" s="5">
         <v>170</v>
       </c>
@@ -818,62 +858,73 @@
         <v>3</v>
       </c>
       <c r="M4" s="5">
-        <v>3</v>
+        <f t="shared" si="0"/>
+        <v>98.6</v>
       </c>
       <c r="N4" s="5">
-        <f t="shared" ref="N4:T4" si="1">N2-0.5</f>
+        <f t="shared" si="1"/>
+        <v>5916</v>
+      </c>
+      <c r="O4" s="5">
+        <v>3</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:V4" si="3">P2-0.5</f>
         <v>1.5</v>
       </c>
-      <c r="O4" s="5">
-        <f t="shared" si="1"/>
+      <c r="Q4" s="5">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="P4" s="5">
-        <f t="shared" si="1"/>
+      <c r="R4" s="5">
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="1"/>
+      <c r="S4" s="5">
+        <f t="shared" si="3"/>
         <v>4.5</v>
       </c>
-      <c r="R4" s="5">
-        <f t="shared" si="1"/>
+      <c r="T4" s="5">
+        <f t="shared" si="3"/>
         <v>3.5</v>
       </c>
-      <c r="S4" s="5">
-        <f t="shared" si="1"/>
+      <c r="U4" s="5">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="T4" s="5">
-        <f t="shared" si="1"/>
+      <c r="V4" s="5">
+        <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="U4" s="5">
+      <c r="W4" s="5">
         <v>2</v>
       </c>
-      <c r="V4" s="5">
-        <v>3</v>
-      </c>
-      <c r="W4" s="5">
-        <v>4</v>
-      </c>
       <c r="X4" s="5">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Y4" s="5">
         <v>4</v>
       </c>
       <c r="Z4" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="AA4" s="5">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
       </c>
+      <c r="D5" s="5">
+        <v>65</v>
+      </c>
       <c r="E5" s="5">
         <v>160</v>
       </c>
@@ -889,14 +940,25 @@
       <c r="I5" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M5" s="5">
+        <f t="shared" si="0"/>
+        <v>92.8</v>
+      </c>
+      <c r="N5" s="5">
+        <f t="shared" si="1"/>
+        <v>6032</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="5">
+        <v>65</v>
+      </c>
       <c r="E6" s="5">
         <v>155</v>
       </c>
@@ -912,14 +974,25 @@
       <c r="I6" s="5">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M6" s="5">
+        <f t="shared" si="0"/>
+        <v>89.899999999999991</v>
+      </c>
+      <c r="N6" s="5">
+        <f t="shared" si="1"/>
+        <v>5843.4999999999991</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>15</v>
       </c>
+      <c r="D7" s="5">
+        <v>66</v>
+      </c>
       <c r="E7" s="5">
         <v>147</v>
       </c>
@@ -932,14 +1005,25 @@
       <c r="I7" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M7" s="5">
+        <f t="shared" si="0"/>
+        <v>85.259999999999991</v>
+      </c>
+      <c r="N7" s="5">
+        <f t="shared" si="1"/>
+        <v>5627.16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
+      <c r="D8" s="5">
+        <v>67</v>
+      </c>
       <c r="E8" s="5">
         <v>139</v>
       </c>
@@ -952,14 +1036,25 @@
       <c r="I8" s="5">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M8" s="5">
+        <f t="shared" si="0"/>
+        <v>80.61999999999999</v>
+      </c>
+      <c r="N8" s="5">
+        <f t="shared" si="1"/>
+        <v>5401.5399999999991</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
+      <c r="D9" s="5">
+        <v>68</v>
+      </c>
       <c r="E9" s="5">
         <v>131</v>
       </c>
@@ -969,14 +1064,25 @@
       <c r="I9" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M9" s="5">
+        <f t="shared" si="0"/>
+        <v>75.97999999999999</v>
+      </c>
+      <c r="N9" s="5">
+        <f t="shared" si="1"/>
+        <v>5166.6399999999994</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
       </c>
+      <c r="D10" s="5">
+        <v>69</v>
+      </c>
       <c r="E10" s="5">
         <v>123</v>
       </c>
@@ -989,14 +1095,25 @@
       <c r="I10" s="5">
         <v>55</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M10" s="5">
+        <f t="shared" si="0"/>
+        <v>71.339999999999989</v>
+      </c>
+      <c r="N10" s="5">
+        <f t="shared" si="1"/>
+        <v>4922.4599999999991</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>16</v>
       </c>
+      <c r="D11" s="5">
+        <v>70</v>
+      </c>
       <c r="E11" s="5">
         <v>115</v>
       </c>
@@ -1006,14 +1123,25 @@
       <c r="I11" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M11" s="5">
+        <f t="shared" si="0"/>
+        <v>66.699999999999989</v>
+      </c>
+      <c r="N11" s="5">
+        <f t="shared" si="1"/>
+        <v>4668.9999999999991</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>16</v>
       </c>
+      <c r="D12" s="5">
+        <v>71</v>
+      </c>
       <c r="E12" s="5">
         <v>107</v>
       </c>
@@ -1026,14 +1154,25 @@
       <c r="H12" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M12" s="5">
+        <f t="shared" si="0"/>
+        <v>62.059999999999995</v>
+      </c>
+      <c r="N12" s="5">
+        <f t="shared" si="1"/>
+        <v>4406.2599999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
         <v>16</v>
       </c>
+      <c r="D13" s="5">
+        <v>72</v>
+      </c>
       <c r="E13" s="5">
         <v>99</v>
       </c>
@@ -1046,16 +1185,35 @@
       <c r="I13" s="5">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="M13" s="5">
+        <f t="shared" si="0"/>
+        <v>57.419999999999995</v>
+      </c>
+      <c r="N13" s="5">
+        <f t="shared" si="1"/>
+        <v>4134.24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
+      <c r="D14" s="5">
+        <v>73</v>
+      </c>
       <c r="E14" s="5">
         <v>91</v>
+      </c>
+      <c r="M14" s="5">
+        <f t="shared" si="0"/>
+        <v>52.779999999999994</v>
+      </c>
+      <c r="N14" s="5">
+        <f t="shared" si="1"/>
+        <v>3852.9399999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just updates to sailor profile to do
</commit_message>
<xml_diff>
--- a/master_c4g_24.xlsx
+++ b/master_c4g_24.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakefarren-price/Google Drive/RYA - Analysis/Crew4Gold_24/c4g/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD9F33F-8D4F-0B4A-B0F6-9644831FAA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADBC3C75-1545-064B-A58D-F7453989B551}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="13380" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="5" r:id="rId5"/>
+    <pivotCache cacheId="1" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>Height</t>
   </si>
   <si>
-    <t>CMJ</t>
-  </si>
-  <si>
     <t>Leg Press</t>
   </si>
   <si>
@@ -350,23 +347,56 @@
     <t>Behaviour Rank</t>
   </si>
   <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>Uni</t>
-  </si>
-  <si>
     <t>Fitness Rank</t>
   </si>
   <si>
     <t>Partner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  01/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12/01/2003</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13/01/2003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -417,6 +447,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -497,7 +533,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -562,7 +598,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -581,8 +616,18 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3106,7 +3151,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3200E97E-E608-2941-A9E2-A293371AF9A7}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3200E97E-E608-2941-A9E2-A293371AF9A7}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:O16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -3292,7 +3337,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95A770F9-FC95-F442-B2CC-40B5FC752FC4}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95A770F9-FC95-F442-B2CC-40B5FC752FC4}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -3932,11 +3977,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:AI14"/>
+  <dimension ref="A1:AH40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="G19" sqref="G19"/>
+      <selection pane="topRight" activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3946,21 +3991,21 @@
     <col min="3" max="3" width="15" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" style="9" customWidth="1"/>
     <col min="5" max="6" width="15" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="15" style="9" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" style="9" customWidth="1"/>
-    <col min="15" max="16" width="15" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="18" max="24" width="15" style="14" bestFit="1" customWidth="1"/>
-    <col min="25" max="30" width="15" style="13" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="21.1640625" style="9" customWidth="1"/>
-    <col min="32" max="32" width="17.1640625" customWidth="1"/>
-    <col min="33" max="33" width="17.5" customWidth="1"/>
-    <col min="34" max="34" width="19.33203125" customWidth="1"/>
-    <col min="35" max="35" width="13.5" customWidth="1"/>
+    <col min="7" max="9" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="15" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="9" customWidth="1"/>
+    <col min="14" max="15" width="15" style="16" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="23" width="15" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="29" width="15" style="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.1640625" style="9" customWidth="1"/>
+    <col min="31" max="31" width="17.1640625" customWidth="1"/>
+    <col min="32" max="32" width="17.5" customWidth="1"/>
+    <col min="33" max="33" width="19.33203125" customWidth="1"/>
+    <col min="34" max="34" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="96" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3971,7 +4016,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -3988,7 +4033,7 @@
       <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
       <c r="K1" s="4" t="s">
@@ -3997,19 +4042,19 @@
       <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="29" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="5" t="s">
         <v>11</v>
-      </c>
-      <c r="N1" s="30" t="s">
-        <v>105</v>
       </c>
       <c r="O1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="R1" s="7" t="s">
@@ -4030,7 +4075,7 @@
       <c r="W1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="X1" s="8" t="s">
         <v>21</v>
       </c>
       <c r="Y1" s="8" t="s">
@@ -4048,1313 +4093,1368 @@
       <c r="AC1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="AD1" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE1" s="27" t="s">
+      <c r="AD1" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="AE1" s="26" t="s">
         <v>99</v>
       </c>
-      <c r="AF1" s="27" t="s">
+      <c r="AF1" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="AG1" s="29" t="s">
+      <c r="AG1" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="AH1" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="20" t="s">
-        <v>76</v>
+      <c r="AH1" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="34" t="s">
+        <v>75</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="12">
-        <v>37622</v>
-      </c>
-      <c r="D2" s="31">
+        <v>35</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="30">
+        <v>68.95</v>
+      </c>
+      <c r="F2" s="30">
+        <v>170.8</v>
+      </c>
+      <c r="G2" s="32">
+        <v>4.5</v>
+      </c>
+      <c r="H2" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="I2" s="32">
+        <v>3.6</v>
+      </c>
+      <c r="L2" s="31">
+        <v>0.91</v>
+      </c>
+      <c r="M2" s="9">
+        <f>_xlfn.RANK.AVG(L2,$L$2:$L$14)</f>
         <v>1</v>
       </c>
-      <c r="E2" s="10">
+      <c r="N2" s="11">
+        <f>0.58*F2</f>
+        <v>99.063999999999993</v>
+      </c>
+      <c r="O2" s="11">
+        <f>N2*E2/100</f>
+        <v>68.304628000000008</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2">
+        <v>3</v>
+      </c>
+      <c r="R2">
+        <v>3</v>
+      </c>
+      <c r="S2">
+        <v>4</v>
+      </c>
+      <c r="T2">
+        <v>4</v>
+      </c>
+      <c r="U2">
+        <v>3</v>
+      </c>
+      <c r="V2">
+        <v>3</v>
+      </c>
+      <c r="W2">
+        <v>4</v>
+      </c>
+      <c r="X2">
+        <v>4</v>
+      </c>
+      <c r="Y2">
+        <v>4</v>
+      </c>
+      <c r="Z2">
+        <v>3</v>
+      </c>
+      <c r="AA2">
+        <v>2</v>
+      </c>
+      <c r="AB2">
+        <v>3</v>
+      </c>
+      <c r="AC2">
+        <v>3</v>
+      </c>
+      <c r="AD2" s="27">
+        <f>AVERAGE(P2:W2)</f>
+        <v>3.375</v>
+      </c>
+      <c r="AE2" s="27">
+        <f>AVERAGE(X2:AC2)</f>
+        <v>3.1666666666666665</v>
+      </c>
+      <c r="AF2" s="9">
+        <f t="shared" ref="AF2:AF11" si="0">_xlfn.RANK.AVG(AD2,$AD$2:$AD$14)</f>
+        <v>11</v>
+      </c>
+      <c r="AG2" s="9">
+        <f t="shared" ref="AG2:AG11" si="1">_xlfn.RANK.AVG(AE2,$AE$2:$AE$14)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E3" s="30">
+        <v>71.5</v>
+      </c>
+      <c r="F3" s="30">
+        <v>173</v>
+      </c>
+      <c r="G3" s="32">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H3" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="I3" s="32">
+        <v>3.3</v>
+      </c>
+      <c r="L3" s="31">
+        <v>0.73</v>
+      </c>
+      <c r="M3" s="9">
+        <f t="shared" ref="M3:M14" si="2">_xlfn.RANK.AVG(L3,$L$2:$L$14)</f>
+        <v>5</v>
+      </c>
+      <c r="N3" s="11">
+        <f t="shared" ref="N3:N14" si="3">0.58*F3</f>
+        <v>100.33999999999999</v>
+      </c>
+      <c r="O3" s="11">
+        <f t="shared" ref="O3:O14" si="4">N3*E3/100</f>
+        <v>71.743099999999998</v>
+      </c>
+      <c r="P3">
+        <v>3.5</v>
+      </c>
+      <c r="Q3">
+        <v>3</v>
+      </c>
+      <c r="R3">
+        <v>3.5</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>3.5</v>
+      </c>
+      <c r="U3">
+        <v>3.5</v>
+      </c>
+      <c r="V3">
+        <v>3.5</v>
+      </c>
+      <c r="W3">
+        <v>3.5</v>
+      </c>
+      <c r="X3">
+        <v>4</v>
+      </c>
+      <c r="Y3">
+        <v>3</v>
+      </c>
+      <c r="Z3">
+        <v>4</v>
+      </c>
+      <c r="AA3">
+        <v>4</v>
+      </c>
+      <c r="AB3">
+        <v>4</v>
+      </c>
+      <c r="AC3">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="27">
+        <f t="shared" ref="AD3:AD14" si="5">AVERAGE(P3:W3)</f>
+        <v>3.5</v>
+      </c>
+      <c r="AE3" s="27">
+        <f t="shared" ref="AE3:AE14" si="6">AVERAGE(X3:AC3)</f>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="AF3" s="9">
+        <f t="shared" si="0"/>
+        <v>9.5</v>
+      </c>
+      <c r="AG3" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="E4" s="30">
+        <v>56.9</v>
+      </c>
+      <c r="F4" s="30">
+        <v>168</v>
+      </c>
+      <c r="G4" s="32">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="H4" s="32">
+        <v>1</v>
+      </c>
+      <c r="I4" s="32">
+        <v>4</v>
+      </c>
+      <c r="L4" s="31">
+        <v>0.9</v>
+      </c>
+      <c r="M4" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" si="3"/>
+        <v>97.44</v>
+      </c>
+      <c r="O4" s="11">
+        <f t="shared" si="4"/>
+        <v>55.443359999999991</v>
+      </c>
+      <c r="P4">
+        <v>3.5</v>
+      </c>
+      <c r="Q4">
+        <v>4</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>4</v>
+      </c>
+      <c r="T4">
+        <v>3.5</v>
+      </c>
+      <c r="U4">
+        <v>3.5</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>4</v>
+      </c>
+      <c r="X4">
+        <v>3.5</v>
+      </c>
+      <c r="Y4">
+        <v>4</v>
+      </c>
+      <c r="Z4">
+        <v>4</v>
+      </c>
+      <c r="AA4">
+        <v>4.5</v>
+      </c>
+      <c r="AB4">
+        <v>4</v>
+      </c>
+      <c r="AC4">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="27">
+        <f t="shared" si="5"/>
+        <v>3.6875</v>
+      </c>
+      <c r="AE4" s="27">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AF4" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="AG4" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="E5" s="30">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="F5" s="30">
+        <v>167.1</v>
+      </c>
+      <c r="G5" s="32">
+        <v>3.7</v>
+      </c>
+      <c r="H5" s="32">
+        <v>1</v>
+      </c>
+      <c r="I5" s="32">
+        <v>3.7</v>
+      </c>
+      <c r="L5" s="31">
+        <v>0.8</v>
+      </c>
+      <c r="M5" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="3"/>
+        <v>96.917999999999992</v>
+      </c>
+      <c r="O5" s="11">
+        <f t="shared" si="4"/>
+        <v>66.00115799999999</v>
+      </c>
+      <c r="P5">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>5</v>
+      </c>
+      <c r="R5">
+        <v>4</v>
+      </c>
+      <c r="S5">
+        <v>5</v>
+      </c>
+      <c r="T5">
+        <v>4</v>
+      </c>
+      <c r="U5">
+        <v>4</v>
+      </c>
+      <c r="V5">
+        <v>5</v>
+      </c>
+      <c r="W5">
+        <v>3</v>
+      </c>
+      <c r="X5">
+        <v>4</v>
+      </c>
+      <c r="Y5">
+        <v>4</v>
+      </c>
+      <c r="Z5">
+        <v>3</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+      <c r="AB5">
+        <v>4</v>
+      </c>
+      <c r="AC5">
+        <v>3</v>
+      </c>
+      <c r="AD5" s="27">
+        <f t="shared" si="5"/>
+        <v>4.25</v>
+      </c>
+      <c r="AE5" s="27">
+        <f t="shared" si="6"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="AF5" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="AG5" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="E6" s="30">
+        <v>70.3</v>
+      </c>
+      <c r="F6" s="30">
+        <v>168.5</v>
+      </c>
+      <c r="G6" s="32">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="H6" s="32">
+        <v>0.9</v>
+      </c>
+      <c r="I6" s="32">
+        <v>3.4</v>
+      </c>
+      <c r="L6" s="31">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="3"/>
+        <v>97.72999999999999</v>
+      </c>
+      <c r="O6" s="11">
+        <f t="shared" si="4"/>
+        <v>68.704189999999983</v>
+      </c>
+      <c r="P6">
+        <v>4</v>
+      </c>
+      <c r="Q6">
+        <v>4</v>
+      </c>
+      <c r="R6">
+        <v>4</v>
+      </c>
+      <c r="S6">
+        <v>4</v>
+      </c>
+      <c r="T6">
+        <v>4</v>
+      </c>
+      <c r="U6">
+        <v>5</v>
+      </c>
+      <c r="V6">
+        <v>5</v>
+      </c>
+      <c r="W6">
+        <v>3</v>
+      </c>
+      <c r="X6">
+        <v>4</v>
+      </c>
+      <c r="Y6">
+        <v>4</v>
+      </c>
+      <c r="Z6">
+        <v>4</v>
+      </c>
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>4</v>
+      </c>
+      <c r="AC6">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="27">
+        <f t="shared" si="5"/>
+        <v>4.125</v>
+      </c>
+      <c r="AE6" s="27">
+        <f t="shared" si="6"/>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="AF6" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="AG6" s="9">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="30">
+        <v>63.35</v>
+      </c>
+      <c r="F7" s="30">
+        <v>164.1</v>
+      </c>
+      <c r="G7" s="32">
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I7" s="32">
+        <v>0</v>
+      </c>
+      <c r="L7" s="31">
+        <v>0.79</v>
+      </c>
+      <c r="M7" s="9">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="3"/>
+        <v>95.177999999999983</v>
+      </c>
+      <c r="O7" s="11">
+        <f t="shared" si="4"/>
+        <v>60.295262999999984</v>
+      </c>
+      <c r="P7">
+        <v>4</v>
+      </c>
+      <c r="Q7">
+        <v>4</v>
+      </c>
+      <c r="R7">
+        <v>4</v>
+      </c>
+      <c r="S7">
+        <v>5</v>
+      </c>
+      <c r="T7">
+        <v>5</v>
+      </c>
+      <c r="U7">
+        <v>4</v>
+      </c>
+      <c r="V7">
+        <v>5</v>
+      </c>
+      <c r="W7">
+        <v>4</v>
+      </c>
+      <c r="X7">
+        <v>5</v>
+      </c>
+      <c r="Y7">
+        <v>4</v>
+      </c>
+      <c r="Z7">
+        <v>4</v>
+      </c>
+      <c r="AA7">
+        <v>4</v>
+      </c>
+      <c r="AB7">
+        <v>5</v>
+      </c>
+      <c r="AC7">
+        <v>4</v>
+      </c>
+      <c r="AD7" s="27">
+        <f t="shared" si="5"/>
+        <v>4.375</v>
+      </c>
+      <c r="AE7" s="27">
+        <f t="shared" si="6"/>
+        <v>4.333333333333333</v>
+      </c>
+      <c r="AF7" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="AG7" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="30">
+        <v>62.35</v>
+      </c>
+      <c r="F8" s="30">
+        <v>168.3</v>
+      </c>
+      <c r="G8" s="32">
+        <v>0</v>
+      </c>
+      <c r="H8" s="32">
+        <v>0.7</v>
+      </c>
+      <c r="I8" s="32">
+        <v>3.4</v>
+      </c>
+      <c r="L8" s="31">
+        <v>0.7</v>
+      </c>
+      <c r="M8" s="9">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="3"/>
+        <v>97.614000000000004</v>
+      </c>
+      <c r="O8" s="11">
+        <f t="shared" si="4"/>
+        <v>60.862329000000003</v>
+      </c>
+      <c r="P8">
+        <v>5</v>
+      </c>
+      <c r="Q8">
+        <v>3</v>
+      </c>
+      <c r="R8">
+        <v>4</v>
+      </c>
+      <c r="S8">
+        <v>3</v>
+      </c>
+      <c r="T8">
+        <v>4</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <v>3</v>
+      </c>
+      <c r="W8">
+        <v>3</v>
+      </c>
+      <c r="X8">
+        <v>5</v>
+      </c>
+      <c r="Y8">
+        <v>4</v>
+      </c>
+      <c r="Z8">
+        <v>4</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AB8">
+        <v>4</v>
+      </c>
+      <c r="AC8">
+        <v>3</v>
+      </c>
+      <c r="AD8" s="27">
+        <f t="shared" si="5"/>
+        <v>3.625</v>
+      </c>
+      <c r="AE8" s="27">
+        <f t="shared" si="6"/>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="AF8" s="9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="AG8" s="9">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="E9" s="30">
+        <v>72.05</v>
+      </c>
+      <c r="F9" s="30">
+        <v>176.6</v>
+      </c>
+      <c r="G9" s="32">
+        <v>4</v>
+      </c>
+      <c r="H9" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I9" s="32">
+        <v>3.4</v>
+      </c>
+      <c r="L9" s="31">
+        <v>0.65</v>
+      </c>
+      <c r="M9" s="9">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="3"/>
+        <v>102.42799999999998</v>
+      </c>
+      <c r="O9" s="11">
+        <f t="shared" si="4"/>
+        <v>73.799373999999986</v>
+      </c>
+      <c r="P9">
+        <v>4</v>
+      </c>
+      <c r="Q9">
+        <v>3</v>
+      </c>
+      <c r="R9">
+        <v>4</v>
+      </c>
+      <c r="S9">
+        <v>4</v>
+      </c>
+      <c r="T9">
+        <v>4</v>
+      </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <v>4</v>
+      </c>
+      <c r="W9">
+        <v>3</v>
+      </c>
+      <c r="X9">
+        <v>4</v>
+      </c>
+      <c r="Y9">
+        <v>3</v>
+      </c>
+      <c r="Z9">
+        <v>4</v>
+      </c>
+      <c r="AA9">
+        <v>3</v>
+      </c>
+      <c r="AB9">
+        <v>4</v>
+      </c>
+      <c r="AC9">
+        <v>5</v>
+      </c>
+      <c r="AD9" s="27">
+        <f t="shared" si="5"/>
+        <v>3.625</v>
+      </c>
+      <c r="AE9" s="27">
+        <f t="shared" si="6"/>
+        <v>3.8333333333333335</v>
+      </c>
+      <c r="AF9" s="9">
+        <f t="shared" si="0"/>
+        <v>7.5</v>
+      </c>
+      <c r="AG9" s="9">
+        <f t="shared" si="1"/>
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="E10" s="33">
         <v>65</v>
       </c>
-      <c r="F2" s="10">
-        <v>180</v>
-      </c>
-      <c r="G2" s="10">
-        <v>1</v>
-      </c>
-      <c r="H2" s="10">
-        <v>2</v>
-      </c>
-      <c r="I2" s="10">
-        <v>23</v>
-      </c>
-      <c r="J2" s="10">
-        <v>356</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="M2" s="9">
-        <v>50</v>
-      </c>
-      <c r="N2" s="9">
-        <f>_xlfn.RANK.AVG(M2,$M$2:$M$14)</f>
-        <v>13</v>
-      </c>
-      <c r="O2" s="11">
-        <f t="shared" ref="O2:O14" si="0">0.58*F2</f>
-        <v>104.39999999999999</v>
-      </c>
-      <c r="P2" s="11">
-        <f>O2*E2/100</f>
-        <v>67.859999999999985</v>
-      </c>
-      <c r="Q2" s="24">
-        <v>3</v>
-      </c>
-      <c r="R2" s="24">
-        <v>3</v>
-      </c>
-      <c r="S2" s="24">
-        <v>3</v>
-      </c>
-      <c r="T2" s="24">
-        <v>4</v>
-      </c>
-      <c r="U2" s="24">
-        <v>4</v>
-      </c>
-      <c r="V2" s="24">
-        <v>3</v>
-      </c>
-      <c r="W2" s="24">
-        <v>3</v>
-      </c>
-      <c r="X2" s="24">
-        <v>4</v>
-      </c>
-      <c r="Y2" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z2" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="24">
-        <v>3</v>
-      </c>
-      <c r="AB2" s="24">
-        <v>2</v>
-      </c>
-      <c r="AC2" s="24">
-        <v>3</v>
-      </c>
-      <c r="AD2" s="24">
-        <v>3</v>
-      </c>
-      <c r="AE2" s="28">
-        <f>AVERAGE(Q2:X2)</f>
-        <v>3.375</v>
-      </c>
-      <c r="AF2" s="28">
-        <f>AVERAGE(Y2:AD2)</f>
-        <v>3.1666666666666665</v>
-      </c>
-      <c r="AG2" s="9">
-        <f>_xlfn.RANK.AVG(AE2,$AE$2:$AE$14)</f>
-        <v>11</v>
-      </c>
-      <c r="AH2" s="9">
-        <f>_xlfn.RANK.AVG(AF2,$AF$2:$AF$14)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="12">
-        <v>37623</v>
-      </c>
-      <c r="D3" s="31">
-        <v>1</v>
-      </c>
-      <c r="E3" s="10">
-        <v>70</v>
-      </c>
-      <c r="F3" s="10">
+      <c r="F10" s="33">
         <v>165</v>
       </c>
-      <c r="G3" s="10">
-        <v>2</v>
-      </c>
-      <c r="H3" s="10">
-        <v>3</v>
-      </c>
-      <c r="I3" s="10">
-        <v>45</v>
-      </c>
-      <c r="J3" s="10">
-        <v>3</v>
-      </c>
-      <c r="M3" s="9">
-        <v>60</v>
-      </c>
-      <c r="N3" s="9">
-        <f t="shared" ref="N3:N14" si="1">_xlfn.RANK.AVG(M3,$M$2:$M$14)</f>
-        <v>12</v>
-      </c>
-      <c r="O3" s="11">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="N10" s="11">
+        <f t="shared" si="3"/>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="O10" s="11">
+        <f t="shared" si="4"/>
+        <v>62.204999999999991</v>
+      </c>
+      <c r="P10">
+        <v>4</v>
+      </c>
+      <c r="Q10">
+        <v>4</v>
+      </c>
+      <c r="R10">
+        <v>3</v>
+      </c>
+      <c r="S10">
+        <v>3.5</v>
+      </c>
+      <c r="T10">
+        <v>4</v>
+      </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <v>4</v>
+      </c>
+      <c r="W10">
+        <v>3.5</v>
+      </c>
+      <c r="X10">
+        <v>4</v>
+      </c>
+      <c r="Y10">
+        <v>3.5</v>
+      </c>
+      <c r="Z10">
+        <v>3</v>
+      </c>
+      <c r="AA10">
+        <v>4</v>
+      </c>
+      <c r="AB10">
+        <v>3</v>
+      </c>
+      <c r="AC10">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="27">
+        <f t="shared" si="5"/>
+        <v>3.75</v>
+      </c>
+      <c r="AE10" s="27">
+        <f t="shared" si="6"/>
+        <v>3.5833333333333335</v>
+      </c>
+      <c r="AF10" s="9">
         <f t="shared" si="0"/>
-        <v>95.699999999999989</v>
-      </c>
-      <c r="P3" s="11">
-        <f t="shared" ref="P3:P14" si="2">O3*E3/100</f>
-        <v>66.989999999999995</v>
-      </c>
-      <c r="Q3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="R3" s="24">
-        <v>3</v>
-      </c>
-      <c r="S3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="T3" s="24">
-        <v>4</v>
-      </c>
-      <c r="U3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="V3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="W3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="X3" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="Y3" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z3" s="24">
-        <v>3</v>
-      </c>
-      <c r="AA3" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB3" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC3" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD3" s="24">
-        <v>3</v>
-      </c>
-      <c r="AE3" s="28">
-        <f t="shared" ref="AE3:AE14" si="3">AVERAGE(Q3:X3)</f>
-        <v>3.5</v>
-      </c>
-      <c r="AF3" s="28">
-        <f t="shared" ref="AF3:AF14" si="4">AVERAGE(Y3:AD3)</f>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="AG3" s="9">
-        <f>_xlfn.RANK.AVG(AE3,$AE$2:$AE$14)</f>
-        <v>9.5</v>
-      </c>
-      <c r="AH3" s="9">
-        <f>_xlfn.RANK.AVG(AF3,$AF$2:$AF$14)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="12">
-        <v>37624</v>
-      </c>
-      <c r="D4" s="31">
-        <v>1</v>
-      </c>
-      <c r="E4" s="10">
-        <v>60</v>
-      </c>
-      <c r="F4" s="10">
-        <v>170</v>
-      </c>
-      <c r="G4" s="10">
-        <v>4</v>
-      </c>
-      <c r="H4" s="10">
         <v>5</v>
       </c>
-      <c r="I4" s="10">
-        <v>6</v>
-      </c>
-      <c r="J4" s="10">
-        <v>3</v>
-      </c>
-      <c r="M4" s="9">
-        <v>70</v>
-      </c>
-      <c r="N4" s="9">
+      <c r="AG10" s="9">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="O4" s="11">
+    </row>
+    <row r="11" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="E11" s="33">
+        <v>65</v>
+      </c>
+      <c r="F11" s="33">
+        <v>165</v>
+      </c>
+      <c r="G11" s="13"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="N11" s="11">
+        <f t="shared" si="3"/>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="O11" s="11">
+        <f t="shared" si="4"/>
+        <v>62.204999999999991</v>
+      </c>
+      <c r="P11">
+        <v>2</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>3</v>
+      </c>
+      <c r="T11">
+        <v>3</v>
+      </c>
+      <c r="U11">
+        <v>3</v>
+      </c>
+      <c r="V11">
+        <v>3</v>
+      </c>
+      <c r="W11">
+        <v>3</v>
+      </c>
+      <c r="X11">
+        <v>4</v>
+      </c>
+      <c r="Y11">
+        <v>3</v>
+      </c>
+      <c r="Z11">
+        <v>4</v>
+      </c>
+      <c r="AA11">
+        <v>4</v>
+      </c>
+      <c r="AB11">
+        <v>3</v>
+      </c>
+      <c r="AC11">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="27">
+        <f t="shared" si="5"/>
+        <v>2.625</v>
+      </c>
+      <c r="AE11" s="27">
+        <f t="shared" si="6"/>
+        <v>3.6666666666666665</v>
+      </c>
+      <c r="AF11" s="9">
         <f t="shared" si="0"/>
-        <v>98.6</v>
-      </c>
-      <c r="P4" s="11">
-        <f t="shared" si="2"/>
-        <v>59.16</v>
-      </c>
-      <c r="Q4" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="R4" s="24">
-        <v>4</v>
-      </c>
-      <c r="S4" s="24">
-        <v>3</v>
-      </c>
-      <c r="T4" s="24">
-        <v>4</v>
-      </c>
-      <c r="U4" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="V4" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="W4" s="24">
-        <v>4</v>
-      </c>
-      <c r="X4" s="24">
-        <v>4</v>
-      </c>
-      <c r="Y4" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="Z4" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA4" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="24">
-        <v>4.5</v>
-      </c>
-      <c r="AC4" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD4" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE4" s="28">
-        <f t="shared" si="3"/>
-        <v>3.6875</v>
-      </c>
-      <c r="AF4" s="28">
-        <f t="shared" si="4"/>
-        <v>4</v>
-      </c>
-      <c r="AG4" s="9">
-        <f>_xlfn.RANK.AVG(AE4,$AE$2:$AE$14)</f>
-        <v>6</v>
-      </c>
-      <c r="AH4" s="9">
-        <f>_xlfn.RANK.AVG(AF4,$AF$2:$AF$14)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C5" s="12">
-        <v>37625</v>
-      </c>
-      <c r="D5" s="31">
-        <v>1</v>
-      </c>
-      <c r="E5" s="10">
-        <v>65</v>
-      </c>
-      <c r="F5" s="10">
-        <v>160</v>
-      </c>
-      <c r="G5" s="10">
-        <v>3</v>
-      </c>
-      <c r="H5" s="10">
-        <v>23</v>
-      </c>
-      <c r="I5" s="10">
-        <v>32</v>
-      </c>
-      <c r="J5" s="10">
-        <v>4</v>
-      </c>
-      <c r="M5" s="9">
-        <v>80</v>
-      </c>
-      <c r="N5" s="9">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="O5" s="11">
-        <f t="shared" si="0"/>
-        <v>92.8</v>
-      </c>
-      <c r="P5" s="11">
-        <f t="shared" si="2"/>
-        <v>60.32</v>
-      </c>
-      <c r="Q5" s="24">
-        <v>4</v>
-      </c>
-      <c r="R5" s="24">
-        <v>5</v>
-      </c>
-      <c r="S5" s="24">
-        <v>4</v>
-      </c>
-      <c r="T5" s="24">
-        <v>5</v>
-      </c>
-      <c r="U5" s="24">
-        <v>4</v>
-      </c>
-      <c r="V5" s="24">
-        <v>4</v>
-      </c>
-      <c r="W5" s="24">
-        <v>5</v>
-      </c>
-      <c r="X5" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y5" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z5" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA5" s="24">
-        <v>3</v>
-      </c>
-      <c r="AB5" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC5" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD5" s="24">
-        <v>3</v>
-      </c>
-      <c r="AE5" s="28">
-        <f t="shared" si="3"/>
-        <v>4.25</v>
-      </c>
-      <c r="AF5" s="28">
-        <f t="shared" si="4"/>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="AG5" s="9">
-        <f>_xlfn.RANK.AVG(AE5,$AE$2:$AE$14)</f>
-        <v>2</v>
-      </c>
-      <c r="AH5" s="9">
-        <f>_xlfn.RANK.AVG(AF5,$AF$2:$AF$14)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="12">
-        <v>37626</v>
-      </c>
-      <c r="D6" s="31">
-        <v>1</v>
-      </c>
-      <c r="E6" s="10">
-        <v>65</v>
-      </c>
-      <c r="F6" s="10">
-        <v>155</v>
-      </c>
-      <c r="G6" s="10">
-        <v>3</v>
-      </c>
-      <c r="H6" s="10">
-        <v>4</v>
-      </c>
-      <c r="I6" s="10">
-        <v>5</v>
-      </c>
-      <c r="J6" s="10">
-        <v>6</v>
-      </c>
-      <c r="M6" s="9">
-        <v>90</v>
-      </c>
-      <c r="N6" s="9">
+        <v>12</v>
+      </c>
+      <c r="AG11" s="9">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="O6" s="11">
-        <f t="shared" si="0"/>
-        <v>89.899999999999991</v>
-      </c>
-      <c r="P6" s="11">
-        <f t="shared" si="2"/>
-        <v>58.434999999999988</v>
-      </c>
-      <c r="Q6" s="24">
-        <v>4</v>
-      </c>
-      <c r="R6" s="24">
-        <v>4</v>
-      </c>
-      <c r="S6" s="24">
-        <v>4</v>
-      </c>
-      <c r="T6" s="24">
-        <v>4</v>
-      </c>
-      <c r="U6" s="24">
-        <v>4</v>
-      </c>
-      <c r="V6" s="24">
-        <v>5</v>
-      </c>
-      <c r="W6" s="24">
-        <v>5</v>
-      </c>
-      <c r="X6" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y6" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z6" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA6" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB6" s="24">
-        <v>3</v>
-      </c>
-      <c r="AC6" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD6" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE6" s="28">
+    </row>
+    <row r="12" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="E12" s="33">
+        <v>65</v>
+      </c>
+      <c r="F12" s="33">
+        <v>165</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="13"/>
+      <c r="N12" s="11">
         <f t="shared" si="3"/>
-        <v>4.125</v>
-      </c>
-      <c r="AF6" s="28">
+        <v>95.699999999999989</v>
+      </c>
+      <c r="O12" s="11">
         <f t="shared" si="4"/>
+        <v>62.204999999999991</v>
+      </c>
+      <c r="AD12" s="27"/>
+      <c r="AE12" s="27"/>
+    </row>
+    <row r="13" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="33">
+        <v>65</v>
+      </c>
+      <c r="F13" s="33">
+        <v>165</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="N13" s="11">
+        <f t="shared" si="3"/>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="O13" s="11">
+        <f t="shared" si="4"/>
+        <v>62.204999999999991</v>
+      </c>
+      <c r="P13">
+        <v>4</v>
+      </c>
+      <c r="Q13">
+        <v>3</v>
+      </c>
+      <c r="R13">
+        <v>3</v>
+      </c>
+      <c r="S13">
+        <v>4</v>
+      </c>
+      <c r="T13">
+        <v>4</v>
+      </c>
+      <c r="U13">
+        <v>3</v>
+      </c>
+      <c r="V13">
+        <v>4</v>
+      </c>
+      <c r="W13">
+        <v>3</v>
+      </c>
+      <c r="X13">
+        <v>4</v>
+      </c>
+      <c r="Y13">
+        <v>4</v>
+      </c>
+      <c r="Z13">
+        <v>4</v>
+      </c>
+      <c r="AA13">
+        <v>4</v>
+      </c>
+      <c r="AB13">
+        <v>3</v>
+      </c>
+      <c r="AC13">
+        <v>4</v>
+      </c>
+      <c r="AD13" s="27">
+        <f t="shared" si="5"/>
+        <v>3.5</v>
+      </c>
+      <c r="AE13" s="27">
+        <f t="shared" si="6"/>
         <v>3.8333333333333335</v>
       </c>
-      <c r="AG6" s="9">
-        <f>_xlfn.RANK.AVG(AE6,$AE$2:$AE$14)</f>
-        <v>3</v>
-      </c>
-      <c r="AH6" s="9">
-        <f>_xlfn.RANK.AVG(AF6,$AF$2:$AF$14)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="12">
-        <v>37627</v>
-      </c>
-      <c r="D7" s="31">
-        <v>1</v>
-      </c>
-      <c r="E7" s="10">
-        <v>66</v>
-      </c>
-      <c r="F7" s="10">
-        <v>147</v>
-      </c>
-      <c r="G7" s="13"/>
-      <c r="H7" s="10">
-        <v>2</v>
-      </c>
-      <c r="I7" s="10">
-        <v>3</v>
-      </c>
-      <c r="J7" s="10">
-        <v>3</v>
-      </c>
-      <c r="M7" s="9">
-        <v>100</v>
-      </c>
-      <c r="N7" s="9">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="O7" s="11">
-        <f t="shared" si="0"/>
-        <v>85.259999999999991</v>
-      </c>
-      <c r="P7" s="11">
-        <f t="shared" si="2"/>
-        <v>56.271599999999999</v>
-      </c>
-      <c r="Q7" s="24">
-        <v>4</v>
-      </c>
-      <c r="R7" s="24">
-        <v>4</v>
-      </c>
-      <c r="S7" s="24">
-        <v>4</v>
-      </c>
-      <c r="T7" s="24">
-        <v>5</v>
-      </c>
-      <c r="U7" s="24">
-        <v>5</v>
-      </c>
-      <c r="V7" s="24">
-        <v>4</v>
-      </c>
-      <c r="W7" s="24">
-        <v>5</v>
-      </c>
-      <c r="X7" s="24">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="24">
-        <v>5</v>
-      </c>
-      <c r="Z7" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA7" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB7" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="24">
-        <v>5</v>
-      </c>
-      <c r="AD7" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE7" s="28">
-        <f t="shared" si="3"/>
-        <v>4.375</v>
-      </c>
-      <c r="AF7" s="28">
-        <f t="shared" si="4"/>
-        <v>4.333333333333333</v>
-      </c>
-      <c r="AG7" s="9">
-        <f>_xlfn.RANK.AVG(AE7,$AE$2:$AE$14)</f>
-        <v>1</v>
-      </c>
-      <c r="AH7" s="9">
-        <f>_xlfn.RANK.AVG(AF7,$AF$2:$AF$14)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="12">
-        <v>37628</v>
-      </c>
-      <c r="D8" s="31">
-        <v>1</v>
-      </c>
-      <c r="E8" s="10">
-        <v>67</v>
-      </c>
-      <c r="F8" s="10">
-        <v>139</v>
-      </c>
-      <c r="G8" s="13"/>
-      <c r="H8" s="10">
-        <v>5</v>
-      </c>
-      <c r="I8" s="10">
-        <v>3</v>
-      </c>
-      <c r="J8" s="10">
-        <v>4</v>
-      </c>
-      <c r="M8" s="9">
-        <v>110</v>
-      </c>
-      <c r="N8" s="9">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="O8" s="11">
-        <f t="shared" si="0"/>
-        <v>80.61999999999999</v>
-      </c>
-      <c r="P8" s="11">
-        <f t="shared" si="2"/>
-        <v>54.015399999999993</v>
-      </c>
-      <c r="Q8" s="24">
-        <v>5</v>
-      </c>
-      <c r="R8" s="24">
-        <v>3</v>
-      </c>
-      <c r="S8" s="24">
-        <v>4</v>
-      </c>
-      <c r="T8" s="24">
-        <v>3</v>
-      </c>
-      <c r="U8" s="24">
-        <v>4</v>
-      </c>
-      <c r="V8" s="24">
-        <v>4</v>
-      </c>
-      <c r="W8" s="24">
-        <v>3</v>
-      </c>
-      <c r="X8" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y8" s="24">
-        <v>5</v>
-      </c>
-      <c r="Z8" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA8" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB8" s="24">
-        <v>3</v>
-      </c>
-      <c r="AC8" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD8" s="24">
-        <v>3</v>
-      </c>
-      <c r="AE8" s="28">
-        <f t="shared" si="3"/>
-        <v>3.625</v>
-      </c>
-      <c r="AF8" s="28">
-        <f t="shared" si="4"/>
-        <v>3.8333333333333335</v>
-      </c>
-      <c r="AG8" s="9">
-        <f>_xlfn.RANK.AVG(AE8,$AE$2:$AE$14)</f>
-        <v>7.5</v>
-      </c>
-      <c r="AH8" s="9">
-        <f>_xlfn.RANK.AVG(AF8,$AF$2:$AF$14)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="12">
-        <v>37629</v>
-      </c>
-      <c r="D9" s="31">
-        <v>1</v>
-      </c>
-      <c r="E9" s="10">
-        <v>68</v>
-      </c>
-      <c r="F9" s="10">
-        <v>131</v>
-      </c>
-      <c r="G9" s="10">
-        <v>5</v>
-      </c>
-      <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
-      <c r="J9" s="10">
-        <v>5</v>
-      </c>
-      <c r="M9" s="9">
-        <v>120</v>
-      </c>
-      <c r="N9" s="9">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="O9" s="11">
-        <f t="shared" si="0"/>
-        <v>75.97999999999999</v>
-      </c>
-      <c r="P9" s="11">
-        <f t="shared" si="2"/>
-        <v>51.666399999999996</v>
-      </c>
-      <c r="Q9" s="24">
-        <v>4</v>
-      </c>
-      <c r="R9" s="24">
-        <v>3</v>
-      </c>
-      <c r="S9" s="24">
-        <v>4</v>
-      </c>
-      <c r="T9" s="24">
-        <v>4</v>
-      </c>
-      <c r="U9" s="24">
-        <v>4</v>
-      </c>
-      <c r="V9" s="24">
-        <v>3</v>
-      </c>
-      <c r="W9" s="24">
-        <v>4</v>
-      </c>
-      <c r="X9" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y9" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z9" s="24">
-        <v>3</v>
-      </c>
-      <c r="AA9" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB9" s="24">
-        <v>3</v>
-      </c>
-      <c r="AC9" s="24">
-        <v>4</v>
-      </c>
-      <c r="AD9" s="24">
-        <v>5</v>
-      </c>
-      <c r="AE9" s="28">
-        <f t="shared" si="3"/>
-        <v>3.625</v>
-      </c>
-      <c r="AF9" s="28">
-        <f t="shared" si="4"/>
-        <v>3.8333333333333335</v>
-      </c>
-      <c r="AG9" s="9">
-        <f>_xlfn.RANK.AVG(AE9,$AE$2:$AE$14)</f>
-        <v>7.5</v>
-      </c>
-      <c r="AH9" s="9">
-        <f>_xlfn.RANK.AVG(AF9,$AF$2:$AF$14)</f>
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B10" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="12">
-        <v>37630</v>
-      </c>
-      <c r="D10" s="31">
-        <v>1</v>
-      </c>
-      <c r="E10" s="10">
-        <v>69</v>
-      </c>
-      <c r="F10" s="10">
-        <v>123</v>
-      </c>
-      <c r="G10" s="13"/>
-      <c r="H10" s="10">
-        <v>5</v>
-      </c>
-      <c r="I10" s="10">
-        <v>6</v>
-      </c>
-      <c r="J10" s="10">
-        <v>55</v>
-      </c>
-      <c r="M10" s="9">
-        <v>130</v>
-      </c>
-      <c r="N10" s="9">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="O10" s="11">
-        <f t="shared" si="0"/>
-        <v>71.339999999999989</v>
-      </c>
-      <c r="P10" s="11">
-        <f t="shared" si="2"/>
-        <v>49.224599999999988</v>
-      </c>
-      <c r="Q10" s="24">
-        <v>4</v>
-      </c>
-      <c r="R10" s="24">
-        <v>4</v>
-      </c>
-      <c r="S10" s="24">
-        <v>3</v>
-      </c>
-      <c r="T10" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="U10" s="24">
-        <v>4</v>
-      </c>
-      <c r="V10" s="24">
-        <v>4</v>
-      </c>
-      <c r="W10" s="24">
-        <v>4</v>
-      </c>
-      <c r="X10" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="Y10" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z10" s="24">
-        <v>3.5</v>
-      </c>
-      <c r="AA10" s="24">
-        <v>3</v>
-      </c>
-      <c r="AB10" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC10" s="24">
-        <v>3</v>
-      </c>
-      <c r="AD10" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE10" s="28">
-        <f t="shared" si="3"/>
-        <v>3.75</v>
-      </c>
-      <c r="AF10" s="28">
-        <f t="shared" si="4"/>
-        <v>3.5833333333333335</v>
-      </c>
-      <c r="AG10" s="9">
-        <f>_xlfn.RANK.AVG(AE10,$AE$2:$AE$14)</f>
-        <v>5</v>
-      </c>
-      <c r="AH10" s="9">
-        <f>_xlfn.RANK.AVG(AF10,$AF$2:$AF$14)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="12">
-        <v>37631</v>
-      </c>
-      <c r="D11" s="31">
-        <v>1</v>
-      </c>
-      <c r="E11" s="10">
-        <v>70</v>
-      </c>
-      <c r="F11" s="10">
-        <v>115</v>
-      </c>
-      <c r="G11" s="13"/>
-      <c r="H11" s="13"/>
-      <c r="I11" s="10">
-        <v>6</v>
-      </c>
-      <c r="J11" s="10">
-        <v>5</v>
-      </c>
-      <c r="M11" s="9">
-        <v>140</v>
-      </c>
-      <c r="N11" s="9">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="O11" s="11">
-        <f t="shared" si="0"/>
-        <v>66.699999999999989</v>
-      </c>
-      <c r="P11" s="11">
-        <f t="shared" si="2"/>
-        <v>46.689999999999991</v>
-      </c>
-      <c r="Q11" s="24">
-        <v>2</v>
-      </c>
-      <c r="R11" s="24">
-        <v>2</v>
-      </c>
-      <c r="S11" s="24">
-        <v>2</v>
-      </c>
-      <c r="T11" s="24">
-        <v>3</v>
-      </c>
-      <c r="U11" s="24">
-        <v>3</v>
-      </c>
-      <c r="V11" s="24">
-        <v>3</v>
-      </c>
-      <c r="W11" s="24">
-        <v>3</v>
-      </c>
-      <c r="X11" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y11" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z11" s="24">
-        <v>3</v>
-      </c>
-      <c r="AA11" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC11" s="24">
-        <v>3</v>
-      </c>
-      <c r="AD11" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE11" s="28">
-        <f t="shared" si="3"/>
-        <v>2.625</v>
-      </c>
-      <c r="AF11" s="28">
-        <f t="shared" si="4"/>
-        <v>3.6666666666666665</v>
-      </c>
-      <c r="AG11" s="9">
-        <f>_xlfn.RANK.AVG(AE11,$AE$2:$AE$14)</f>
-        <v>12</v>
-      </c>
-      <c r="AH11" s="9">
-        <f>_xlfn.RANK.AVG(AF11,$AF$2:$AF$14)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="12">
-        <v>37632</v>
-      </c>
-      <c r="D12" s="31">
-        <v>1</v>
-      </c>
-      <c r="E12" s="10">
-        <v>71</v>
-      </c>
-      <c r="F12" s="10">
-        <v>107</v>
-      </c>
-      <c r="G12" s="10">
-        <v>3</v>
-      </c>
-      <c r="H12" s="10">
-        <v>55</v>
-      </c>
-      <c r="I12" s="10">
-        <v>5</v>
-      </c>
-      <c r="J12" s="13"/>
-      <c r="M12" s="9">
-        <v>150</v>
-      </c>
-      <c r="N12" s="9">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="O12" s="11">
-        <f t="shared" si="0"/>
-        <v>62.059999999999995</v>
-      </c>
-      <c r="P12" s="11">
-        <f t="shared" si="2"/>
-        <v>44.062599999999996</v>
-      </c>
-      <c r="AE12" s="28"/>
-      <c r="AF12" s="28"/>
-    </row>
-    <row r="13" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="12">
-        <v>37633</v>
-      </c>
-      <c r="D13" s="31">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10">
-        <v>72</v>
-      </c>
-      <c r="F13" s="10">
-        <v>99</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="10">
-        <v>3</v>
-      </c>
-      <c r="I13" s="10">
-        <v>3</v>
-      </c>
-      <c r="J13" s="10">
-        <v>3</v>
-      </c>
-      <c r="M13" s="9">
-        <v>160</v>
-      </c>
-      <c r="N13" s="9">
-        <f t="shared" si="1"/>
-        <v>2</v>
-      </c>
-      <c r="O13" s="11">
-        <f t="shared" si="0"/>
-        <v>57.419999999999995</v>
-      </c>
-      <c r="P13" s="11">
-        <f t="shared" si="2"/>
-        <v>41.342399999999998</v>
-      </c>
-      <c r="Q13" s="24">
-        <v>4</v>
-      </c>
-      <c r="R13" s="24">
-        <v>3</v>
-      </c>
-      <c r="S13" s="24">
-        <v>3</v>
-      </c>
-      <c r="T13" s="24">
-        <v>4</v>
-      </c>
-      <c r="U13" s="24">
-        <v>4</v>
-      </c>
-      <c r="V13" s="24">
-        <v>3</v>
-      </c>
-      <c r="W13" s="24">
-        <v>4</v>
-      </c>
-      <c r="X13" s="24">
-        <v>3</v>
-      </c>
-      <c r="Y13" s="24">
-        <v>4</v>
-      </c>
-      <c r="Z13" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA13" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB13" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC13" s="24">
-        <v>3</v>
-      </c>
-      <c r="AD13" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE13" s="28">
-        <f t="shared" si="3"/>
-        <v>3.5</v>
-      </c>
-      <c r="AF13" s="28">
-        <f t="shared" si="4"/>
-        <v>3.8333333333333335</v>
+      <c r="AF13" s="9">
+        <f>_xlfn.RANK.AVG(AD13,$AD$2:$AD$14)</f>
+        <v>9.5</v>
       </c>
       <c r="AG13" s="9">
         <f>_xlfn.RANK.AVG(AE13,$AE$2:$AE$14)</f>
-        <v>9.5</v>
-      </c>
-      <c r="AH13" s="9">
-        <f>_xlfn.RANK.AVG(AF13,$AF$2:$AF$14)</f>
         <v>5.5</v>
       </c>
     </row>
-    <row r="14" spans="1:35" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" s="9" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C14" s="12">
-        <v>37634</v>
-      </c>
-      <c r="D14" s="31">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10">
-        <v>73</v>
-      </c>
-      <c r="F14" s="10">
-        <v>91</v>
-      </c>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
+        <v>28</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="30">
+        <v>71.3</v>
+      </c>
+      <c r="F14" s="30">
+        <v>173</v>
+      </c>
+      <c r="G14" s="32">
+        <v>3.5</v>
+      </c>
+      <c r="H14" s="32">
+        <v>0.8</v>
+      </c>
+      <c r="I14" s="32">
+        <v>3.6</v>
+      </c>
+      <c r="L14" s="31">
+        <v>0.72</v>
+      </c>
       <c r="M14" s="9">
-        <v>170</v>
-      </c>
-      <c r="N14" s="9">
-        <f t="shared" si="1"/>
-        <v>1</v>
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="3"/>
+        <v>100.33999999999999</v>
       </c>
       <c r="O14" s="11">
-        <f t="shared" si="0"/>
-        <v>52.779999999999994</v>
-      </c>
-      <c r="P14" s="11">
-        <f t="shared" si="2"/>
-        <v>38.529399999999995</v>
-      </c>
-      <c r="Q14" s="24">
+        <f t="shared" si="4"/>
+        <v>71.542419999999993</v>
+      </c>
+      <c r="P14">
         <v>5</v>
       </c>
-      <c r="R14" s="24">
-        <v>4</v>
-      </c>
-      <c r="S14" s="24">
-        <v>4</v>
-      </c>
-      <c r="T14" s="24">
+      <c r="Q14">
+        <v>4</v>
+      </c>
+      <c r="R14">
+        <v>4</v>
+      </c>
+      <c r="S14">
         <v>3.5</v>
       </c>
-      <c r="U14" s="24">
-        <v>4</v>
-      </c>
-      <c r="V14" s="24">
+      <c r="T14">
+        <v>4</v>
+      </c>
+      <c r="U14">
         <v>4.5</v>
       </c>
-      <c r="W14" s="24">
+      <c r="V14">
         <v>3.5</v>
       </c>
-      <c r="X14" s="24">
+      <c r="W14">
         <v>3.5</v>
       </c>
-      <c r="Y14" s="24">
+      <c r="X14">
         <v>3.5</v>
       </c>
-      <c r="Z14" s="24">
-        <v>4</v>
-      </c>
-      <c r="AA14" s="24">
-        <v>4</v>
-      </c>
-      <c r="AB14" s="24">
-        <v>4</v>
-      </c>
-      <c r="AC14" s="24">
+      <c r="Y14">
+        <v>4</v>
+      </c>
+      <c r="Z14">
+        <v>4</v>
+      </c>
+      <c r="AA14">
+        <v>4</v>
+      </c>
+      <c r="AB14">
         <v>5</v>
       </c>
-      <c r="AD14" s="24">
-        <v>4</v>
-      </c>
-      <c r="AE14" s="28">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
-      <c r="AF14" s="28">
-        <f t="shared" si="4"/>
+      <c r="AC14">
+        <v>4</v>
+      </c>
+      <c r="AD14" s="27">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AE14" s="27">
+        <f t="shared" si="6"/>
         <v>4.083333333333333</v>
+      </c>
+      <c r="AF14" s="9">
+        <f>_xlfn.RANK.AVG(AD14,$AD$2:$AD$14)</f>
+        <v>4</v>
       </c>
       <c r="AG14" s="9">
         <f>_xlfn.RANK.AVG(AE14,$AE$2:$AE$14)</f>
-        <v>4</v>
-      </c>
-      <c r="AH14" s="9">
-        <f>_xlfn.RANK.AVG(AF14,$AF$2:$AF$14)</f>
         <v>2</v>
       </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="9"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B35" s="9"/>
+      <c r="E35" s="9"/>
+      <c r="F35" s="9"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="9"/>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B36" s="9"/>
+      <c r="E36" s="9"/>
+      <c r="F36" s="9"/>
+      <c r="G36" s="9"/>
+      <c r="H36" s="9"/>
+      <c r="I36" s="9"/>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B37" s="9"/>
+      <c r="E37" s="9"/>
+      <c r="F37" s="9"/>
+      <c r="G37" s="9"/>
+      <c r="H37" s="9"/>
+      <c r="I37" s="9"/>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="9"/>
+      <c r="G38" s="9"/>
+      <c r="H38" s="9"/>
+      <c r="I38" s="9"/>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B39" s="9"/>
+      <c r="E39" s="9"/>
+      <c r="F39" s="9"/>
+      <c r="G39" s="9"/>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B40" s="9"/>
+      <c r="E40" s="9"/>
+      <c r="F40" s="9"/>
+      <c r="G40" s="9"/>
+      <c r="H40" s="9"/>
+      <c r="I40" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5376,660 +5476,660 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:15" s="9" customFormat="1" ht="56" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
-        <v>81</v>
+      <c r="A3" s="24" t="s">
+        <v>80</v>
       </c>
       <c r="B3" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="D3" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="E3" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="F3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="G3" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="H3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="I3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="J3" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="K3" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="L3" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="M3" s="9" t="s">
+      <c r="N3" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="O3" s="9" t="s">
         <v>96</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B4" s="24">
-        <v>3</v>
-      </c>
-      <c r="C4" s="24">
-        <v>3</v>
-      </c>
-      <c r="D4" s="24">
-        <v>3</v>
-      </c>
-      <c r="E4" s="24">
-        <v>4</v>
-      </c>
-      <c r="F4" s="24">
-        <v>4</v>
-      </c>
-      <c r="G4" s="24">
-        <v>3</v>
-      </c>
-      <c r="H4" s="24">
-        <v>3</v>
-      </c>
-      <c r="I4" s="24">
-        <v>4</v>
-      </c>
-      <c r="J4" s="24">
-        <v>4</v>
-      </c>
-      <c r="K4" s="24">
-        <v>4</v>
-      </c>
-      <c r="L4" s="24">
-        <v>3</v>
-      </c>
-      <c r="M4" s="24">
+        <v>75</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <v>3</v>
+      </c>
+      <c r="M4">
         <v>2</v>
       </c>
-      <c r="N4" s="24">
-        <v>3</v>
-      </c>
-      <c r="O4" s="24">
+      <c r="N4">
+        <v>3</v>
+      </c>
+      <c r="O4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="24">
+        <v>32</v>
+      </c>
+      <c r="B5">
         <v>3.5</v>
       </c>
-      <c r="C5" s="24">
-        <v>3</v>
-      </c>
-      <c r="D5" s="24">
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
         <v>3.5</v>
       </c>
-      <c r="E5" s="24">
-        <v>4</v>
-      </c>
-      <c r="F5" s="24">
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
         <v>3.5</v>
       </c>
-      <c r="G5" s="24">
+      <c r="G5">
         <v>3.5</v>
       </c>
-      <c r="H5" s="24">
+      <c r="H5">
         <v>3.5</v>
       </c>
-      <c r="I5" s="24">
+      <c r="I5">
         <v>3.5</v>
       </c>
-      <c r="J5" s="24">
-        <v>4</v>
-      </c>
-      <c r="K5" s="24">
-        <v>3</v>
-      </c>
-      <c r="L5" s="24">
-        <v>4</v>
-      </c>
-      <c r="M5" s="24">
-        <v>4</v>
-      </c>
-      <c r="N5" s="24">
-        <v>4</v>
-      </c>
-      <c r="O5" s="24">
+      <c r="J5">
+        <v>4</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>4</v>
+      </c>
+      <c r="M5">
+        <v>4</v>
+      </c>
+      <c r="N5">
+        <v>4</v>
+      </c>
+      <c r="O5">
         <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="24">
+        <v>58</v>
+      </c>
+      <c r="B6">
         <v>3.5</v>
       </c>
-      <c r="C6" s="24">
-        <v>4</v>
-      </c>
-      <c r="D6" s="24">
-        <v>3</v>
-      </c>
-      <c r="E6" s="24">
-        <v>4</v>
-      </c>
-      <c r="F6" s="24">
+      <c r="C6">
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
         <v>3.5</v>
       </c>
-      <c r="G6" s="24">
+      <c r="G6">
         <v>3.5</v>
       </c>
-      <c r="H6" s="24">
-        <v>4</v>
-      </c>
-      <c r="I6" s="24">
-        <v>4</v>
-      </c>
-      <c r="J6" s="24">
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>4</v>
+      </c>
+      <c r="J6">
         <v>3.5</v>
       </c>
-      <c r="K6" s="24">
-        <v>4</v>
-      </c>
-      <c r="L6" s="24">
-        <v>4</v>
-      </c>
-      <c r="M6" s="24">
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
         <v>4.5</v>
       </c>
-      <c r="N6" s="24">
-        <v>4</v>
-      </c>
-      <c r="O6" s="24">
+      <c r="N6">
+        <v>4</v>
+      </c>
+      <c r="O6">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="24">
-        <v>4</v>
-      </c>
-      <c r="C7" s="24">
+        <v>33</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7">
         <v>5</v>
       </c>
-      <c r="D7" s="24">
-        <v>4</v>
-      </c>
-      <c r="E7" s="24">
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
         <v>5</v>
       </c>
-      <c r="F7" s="24">
-        <v>4</v>
-      </c>
-      <c r="G7" s="24">
-        <v>4</v>
-      </c>
-      <c r="H7" s="24">
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
+      <c r="H7">
         <v>5</v>
       </c>
-      <c r="I7" s="24">
-        <v>3</v>
-      </c>
-      <c r="J7" s="24">
-        <v>4</v>
-      </c>
-      <c r="K7" s="24">
-        <v>4</v>
-      </c>
-      <c r="L7" s="24">
-        <v>3</v>
-      </c>
-      <c r="M7" s="24">
-        <v>4</v>
-      </c>
-      <c r="N7" s="24">
-        <v>4</v>
-      </c>
-      <c r="O7" s="24">
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7">
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <v>4</v>
+      </c>
+      <c r="N7">
+        <v>4</v>
+      </c>
+      <c r="O7">
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="24">
-        <v>4</v>
-      </c>
-      <c r="C8" s="24">
-        <v>4</v>
-      </c>
-      <c r="D8" s="24">
-        <v>4</v>
-      </c>
-      <c r="E8" s="24">
-        <v>4</v>
-      </c>
-      <c r="F8" s="24">
-        <v>4</v>
-      </c>
-      <c r="G8" s="24">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>4</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
         <v>5</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8">
         <v>5</v>
       </c>
-      <c r="I8" s="24">
-        <v>3</v>
-      </c>
-      <c r="J8" s="24">
-        <v>4</v>
-      </c>
-      <c r="K8" s="24">
-        <v>4</v>
-      </c>
-      <c r="L8" s="24">
-        <v>4</v>
-      </c>
-      <c r="M8" s="24">
-        <v>3</v>
-      </c>
-      <c r="N8" s="24">
-        <v>4</v>
-      </c>
-      <c r="O8" s="24">
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>4</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8">
+        <v>4</v>
+      </c>
+      <c r="M8">
+        <v>3</v>
+      </c>
+      <c r="N8">
+        <v>4</v>
+      </c>
+      <c r="O8">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="24">
-        <v>4</v>
-      </c>
-      <c r="C9" s="24">
-        <v>4</v>
-      </c>
-      <c r="D9" s="24">
-        <v>4</v>
-      </c>
-      <c r="E9" s="24">
+        <v>71</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
         <v>5</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9">
         <v>5</v>
       </c>
-      <c r="G9" s="24">
-        <v>4</v>
-      </c>
-      <c r="H9" s="24">
+      <c r="G9">
+        <v>4</v>
+      </c>
+      <c r="H9">
         <v>5</v>
       </c>
-      <c r="I9" s="24">
-        <v>4</v>
-      </c>
-      <c r="J9" s="24">
+      <c r="I9">
+        <v>4</v>
+      </c>
+      <c r="J9">
         <v>5</v>
       </c>
-      <c r="K9" s="24">
-        <v>4</v>
-      </c>
-      <c r="L9" s="24">
-        <v>4</v>
-      </c>
-      <c r="M9" s="24">
-        <v>4</v>
-      </c>
-      <c r="N9" s="24">
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9">
+        <v>4</v>
+      </c>
+      <c r="M9">
+        <v>4</v>
+      </c>
+      <c r="N9">
         <v>5</v>
       </c>
-      <c r="O9" s="24">
+      <c r="O9">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="B10" s="24">
+        <v>34</v>
+      </c>
+      <c r="B10">
         <v>5</v>
       </c>
-      <c r="C10" s="24">
-        <v>3</v>
-      </c>
-      <c r="D10" s="24">
-        <v>4</v>
-      </c>
-      <c r="E10" s="24">
-        <v>3</v>
-      </c>
-      <c r="F10" s="24">
-        <v>4</v>
-      </c>
-      <c r="G10" s="24">
-        <v>4</v>
-      </c>
-      <c r="H10" s="24">
-        <v>3</v>
-      </c>
-      <c r="I10" s="24">
-        <v>3</v>
-      </c>
-      <c r="J10" s="24">
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10">
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
         <v>5</v>
       </c>
-      <c r="K10" s="24">
-        <v>4</v>
-      </c>
-      <c r="L10" s="24">
-        <v>4</v>
-      </c>
-      <c r="M10" s="24">
-        <v>3</v>
-      </c>
-      <c r="N10" s="24">
-        <v>4</v>
-      </c>
-      <c r="O10" s="24">
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10">
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+      <c r="N10">
+        <v>4</v>
+      </c>
+      <c r="O10">
         <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B11" s="24">
-        <v>4</v>
-      </c>
-      <c r="C11" s="24">
-        <v>3</v>
-      </c>
-      <c r="D11" s="24">
-        <v>4</v>
-      </c>
-      <c r="E11" s="24">
-        <v>4</v>
-      </c>
-      <c r="F11" s="24">
-        <v>4</v>
-      </c>
-      <c r="G11" s="24">
-        <v>3</v>
-      </c>
-      <c r="H11" s="24">
-        <v>4</v>
-      </c>
-      <c r="I11" s="24">
-        <v>3</v>
-      </c>
-      <c r="J11" s="24">
-        <v>4</v>
-      </c>
-      <c r="K11" s="24">
-        <v>3</v>
-      </c>
-      <c r="L11" s="24">
-        <v>4</v>
-      </c>
-      <c r="M11" s="24">
-        <v>3</v>
-      </c>
-      <c r="N11" s="24">
-        <v>4</v>
-      </c>
-      <c r="O11" s="24">
+        <v>73</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>3</v>
+      </c>
+      <c r="L11">
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <v>3</v>
+      </c>
+      <c r="N11">
+        <v>4</v>
+      </c>
+      <c r="O11">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B12" s="24">
-        <v>4</v>
-      </c>
-      <c r="C12" s="24">
-        <v>4</v>
-      </c>
-      <c r="D12" s="24">
-        <v>3</v>
-      </c>
-      <c r="E12" s="24">
+        <v>54</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>4</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="E12">
         <v>3.5</v>
       </c>
-      <c r="F12" s="24">
-        <v>4</v>
-      </c>
-      <c r="G12" s="24">
-        <v>4</v>
-      </c>
-      <c r="H12" s="24">
-        <v>4</v>
-      </c>
-      <c r="I12" s="24">
+      <c r="F12">
+        <v>4</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
         <v>3.5</v>
       </c>
-      <c r="J12" s="24">
-        <v>4</v>
-      </c>
-      <c r="K12" s="24">
+      <c r="J12">
+        <v>4</v>
+      </c>
+      <c r="K12">
         <v>3.5</v>
       </c>
-      <c r="L12" s="24">
-        <v>3</v>
-      </c>
-      <c r="M12" s="24">
-        <v>4</v>
-      </c>
-      <c r="N12" s="24">
-        <v>3</v>
-      </c>
-      <c r="O12" s="24">
+      <c r="L12">
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <v>4</v>
+      </c>
+      <c r="N12">
+        <v>3</v>
+      </c>
+      <c r="O12">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="24">
+        <v>27</v>
+      </c>
+      <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13">
         <v>2</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13">
         <v>2</v>
       </c>
-      <c r="E13" s="24">
-        <v>3</v>
-      </c>
-      <c r="F13" s="24">
-        <v>3</v>
-      </c>
-      <c r="G13" s="24">
-        <v>3</v>
-      </c>
-      <c r="H13" s="24">
-        <v>3</v>
-      </c>
-      <c r="I13" s="24">
-        <v>3</v>
-      </c>
-      <c r="J13" s="24">
-        <v>4</v>
-      </c>
-      <c r="K13" s="24">
-        <v>3</v>
-      </c>
-      <c r="L13" s="24">
-        <v>4</v>
-      </c>
-      <c r="M13" s="24">
-        <v>4</v>
-      </c>
-      <c r="N13" s="24">
-        <v>3</v>
-      </c>
-      <c r="O13" s="24">
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
+        <v>4</v>
+      </c>
+      <c r="N13">
+        <v>3</v>
+      </c>
+      <c r="O13">
         <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="24">
-        <v>4</v>
-      </c>
-      <c r="C14" s="24">
-        <v>3</v>
-      </c>
-      <c r="D14" s="24">
-        <v>3</v>
-      </c>
-      <c r="E14" s="24">
-        <v>4</v>
-      </c>
-      <c r="F14" s="24">
-        <v>4</v>
-      </c>
-      <c r="G14" s="24">
-        <v>3</v>
-      </c>
-      <c r="H14" s="24">
-        <v>4</v>
-      </c>
-      <c r="I14" s="24">
-        <v>3</v>
-      </c>
-      <c r="J14" s="24">
-        <v>4</v>
-      </c>
-      <c r="K14" s="24">
-        <v>4</v>
-      </c>
-      <c r="L14" s="24">
-        <v>4</v>
-      </c>
-      <c r="M14" s="24">
-        <v>4</v>
-      </c>
-      <c r="N14" s="24">
-        <v>3</v>
-      </c>
-      <c r="O14" s="24">
+        <v>69</v>
+      </c>
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>4</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14">
+        <v>4</v>
+      </c>
+      <c r="M14">
+        <v>4</v>
+      </c>
+      <c r="N14">
+        <v>3</v>
+      </c>
+      <c r="O14">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="24">
+        <v>30</v>
+      </c>
+      <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="24">
-        <v>4</v>
-      </c>
-      <c r="D15" s="24">
-        <v>4</v>
-      </c>
-      <c r="E15" s="24">
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
         <v>3.5</v>
       </c>
-      <c r="F15" s="24">
-        <v>4</v>
-      </c>
-      <c r="G15" s="24">
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
         <v>4.5</v>
       </c>
-      <c r="H15" s="24">
+      <c r="H15">
         <v>3.5</v>
       </c>
-      <c r="I15" s="24">
+      <c r="I15">
         <v>3.5</v>
       </c>
-      <c r="J15" s="24">
+      <c r="J15">
         <v>3.5</v>
       </c>
-      <c r="K15" s="24">
-        <v>4</v>
-      </c>
-      <c r="L15" s="24">
-        <v>4</v>
-      </c>
-      <c r="M15" s="24">
-        <v>4</v>
-      </c>
-      <c r="N15" s="24">
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+      <c r="N15">
         <v>5</v>
       </c>
-      <c r="O15" s="24">
+      <c r="O15">
         <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="24">
+        <v>82</v>
+      </c>
+      <c r="B16">
         <v>3.8</v>
       </c>
-      <c r="C16" s="24">
+      <c r="C16">
         <v>3.5333333333333332</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16">
         <v>3.4375</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16">
         <v>3.875</v>
       </c>
-      <c r="F16" s="24">
+      <c r="F16">
         <v>3.875</v>
       </c>
-      <c r="G16" s="24">
+      <c r="G16">
         <v>3.75</v>
       </c>
-      <c r="H16" s="24">
+      <c r="H16">
         <v>3.875</v>
       </c>
-      <c r="I16" s="24">
+      <c r="I16">
         <v>3.4375</v>
       </c>
-      <c r="J16" s="24">
-        <v>4</v>
-      </c>
-      <c r="K16" s="24">
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16">
         <v>3.6875</v>
       </c>
-      <c r="L16" s="24">
+      <c r="L16">
         <v>3.75</v>
       </c>
-      <c r="M16" s="24">
+      <c r="M16">
         <v>3.6923076923076925</v>
       </c>
-      <c r="N16" s="24">
+      <c r="N16">
         <v>3.8333333333333335</v>
       </c>
-      <c r="O16" s="24">
+      <c r="O16">
         <v>3.75</v>
       </c>
     </row>
@@ -6053,163 +6153,163 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="24" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A5" s="25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="25" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A7" s="25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A8" s="25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A10" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A11" s="25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="25" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A13" s="25" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="25" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A15" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A17" s="25" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A19" s="25" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="112" x14ac:dyDescent="0.2">
+      <c r="A21" s="25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A23" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A26" s="25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A27" s="25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A28" s="25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A30" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="26" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A5" s="26" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="26" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="26" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A8" s="26" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="26" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A11" s="26" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="26" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A13" s="26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="26" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="26" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="26" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="26" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="26" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="26" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A21" s="26" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="26" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="26" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A25" s="26" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A26" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="26" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="26" t="s">
+    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A33" s="26" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="26" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>
@@ -6232,58 +6332,58 @@
   <sheetData>
     <row r="1" spans="1:24" s="23" customFormat="1" ht="88" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="21" t="s">
+      <c r="D1" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="E1" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="F1" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="21" t="s">
+      <c r="G1" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="21" t="s">
+      <c r="H1" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="21" t="s">
+      <c r="I1" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="J1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="J1" s="21" t="s">
+      <c r="K1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="K1" s="21" t="s">
+      <c r="L1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="L1" s="21" t="s">
+      <c r="M1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="M1" s="21" t="s">
+      <c r="N1" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="N1" s="21" t="s">
+      <c r="O1" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="O1" s="21" t="s">
+      <c r="P1" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="P1" s="21" t="s">
+      <c r="Q1" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="Q1" s="21" t="s">
+      <c r="R1" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="R1" s="21" t="s">
-        <v>53</v>
       </c>
       <c r="S1" s="22"/>
       <c r="T1" s="22"/>
@@ -6297,10 +6397,10 @@
         <v>45636.892523148148</v>
       </c>
       <c r="B2" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="19" t="s">
         <v>54</v>
-      </c>
-      <c r="C2" s="19" t="s">
-        <v>55</v>
       </c>
       <c r="D2" s="19">
         <v>3</v>
@@ -6337,7 +6437,7 @@
       <c r="P2" s="17"/>
       <c r="Q2" s="17"/>
       <c r="R2" s="19" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="S2" s="17"/>
       <c r="T2" s="17"/>
@@ -6351,10 +6451,10 @@
         <v>45636.899305555555</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="17"/>
       <c r="E3" s="17"/>
@@ -6387,7 +6487,7 @@
       <c r="P3" s="17"/>
       <c r="Q3" s="17"/>
       <c r="R3" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S3" s="17"/>
       <c r="T3" s="17"/>
@@ -6401,10 +6501,10 @@
         <v>45636.91138888889</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="19">
         <v>3</v>
@@ -6443,7 +6543,7 @@
       <c r="P4" s="17"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S4" s="17"/>
       <c r="T4" s="17"/>
@@ -6457,10 +6557,10 @@
         <v>45636.918946759259</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" s="19">
         <v>3</v>
@@ -6497,7 +6597,7 @@
       <c r="P5" s="17"/>
       <c r="Q5" s="17"/>
       <c r="R5" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="S5" s="17"/>
       <c r="T5" s="17"/>
@@ -6511,10 +6611,10 @@
         <v>45607.607951388891</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="19">
         <v>2</v>
@@ -6559,7 +6659,7 @@
         <v>4</v>
       </c>
       <c r="R6" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S6" s="17"/>
       <c r="T6" s="17"/>
@@ -6573,10 +6673,10 @@
         <v>45607.612893518519</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="19">
         <v>5</v>
@@ -6621,7 +6721,7 @@
         <v>4</v>
       </c>
       <c r="R7" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="S7" s="17"/>
       <c r="T7" s="17"/>
@@ -6635,10 +6735,10 @@
         <v>45607.616203703707</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D8" s="19">
         <v>4</v>
@@ -6683,7 +6783,7 @@
         <v>4</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="S8" s="17"/>
       <c r="T8" s="17"/>
@@ -6697,10 +6797,10 @@
         <v>45607.722337962965</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D9" s="19">
         <v>4</v>
@@ -6745,7 +6845,7 @@
         <v>3</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="S9" s="17"/>
       <c r="T9" s="17"/>
@@ -6759,10 +6859,10 @@
         <v>45607.726018518515</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="19">
         <v>4</v>
@@ -6807,7 +6907,7 @@
         <v>3</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="S10" s="17"/>
       <c r="T10" s="17"/>
@@ -6821,10 +6921,10 @@
         <v>45607.728530092594</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="19">
         <v>5</v>
@@ -6869,7 +6969,7 @@
         <v>3</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="S11" s="17"/>
       <c r="T11" s="17"/>
@@ -6883,55 +6983,55 @@
         <v>45607.732418981483</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="19">
+        <v>4</v>
+      </c>
+      <c r="E12" s="19">
+        <v>3</v>
+      </c>
+      <c r="F12" s="19">
+        <v>3</v>
+      </c>
+      <c r="G12" s="19">
+        <v>4</v>
+      </c>
+      <c r="H12" s="19">
+        <v>4</v>
+      </c>
+      <c r="I12" s="19">
+        <v>3</v>
+      </c>
+      <c r="J12" s="19">
+        <v>4</v>
+      </c>
+      <c r="K12" s="19">
+        <v>3</v>
+      </c>
+      <c r="L12" s="19">
+        <v>4</v>
+      </c>
+      <c r="M12" s="19">
+        <v>4</v>
+      </c>
+      <c r="N12" s="19">
+        <v>4</v>
+      </c>
+      <c r="O12" s="19">
+        <v>4</v>
+      </c>
+      <c r="P12" s="19">
+        <v>3</v>
+      </c>
+      <c r="Q12" s="19">
+        <v>4</v>
+      </c>
+      <c r="R12" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="D12" s="19">
-        <v>4</v>
-      </c>
-      <c r="E12" s="19">
-        <v>3</v>
-      </c>
-      <c r="F12" s="19">
-        <v>3</v>
-      </c>
-      <c r="G12" s="19">
-        <v>4</v>
-      </c>
-      <c r="H12" s="19">
-        <v>4</v>
-      </c>
-      <c r="I12" s="19">
-        <v>3</v>
-      </c>
-      <c r="J12" s="19">
-        <v>4</v>
-      </c>
-      <c r="K12" s="19">
-        <v>3</v>
-      </c>
-      <c r="L12" s="19">
-        <v>4</v>
-      </c>
-      <c r="M12" s="19">
-        <v>4</v>
-      </c>
-      <c r="N12" s="19">
-        <v>4</v>
-      </c>
-      <c r="O12" s="19">
-        <v>4</v>
-      </c>
-      <c r="P12" s="19">
-        <v>3</v>
-      </c>
-      <c r="Q12" s="19">
-        <v>4</v>
-      </c>
-      <c r="R12" s="19" t="s">
-        <v>71</v>
       </c>
       <c r="S12" s="17"/>
       <c r="T12" s="17"/>
@@ -6945,10 +7045,10 @@
         <v>45607.736215277779</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D13" s="19">
         <v>4</v>
@@ -6993,7 +7093,7 @@
         <v>4</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="S13" s="17"/>
       <c r="T13" s="17"/>
@@ -7007,10 +7107,10 @@
         <v>45607.741226851853</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="19">
         <v>4</v>
@@ -7055,7 +7155,7 @@
         <v>5</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="S14" s="17"/>
       <c r="T14" s="17"/>
@@ -7069,10 +7169,10 @@
         <v>45607.749212962961</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D15" s="19">
         <v>3</v>
@@ -7117,7 +7217,7 @@
         <v>3</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S15" s="17"/>
       <c r="T15" s="17"/>
@@ -7131,10 +7231,10 @@
         <v>45607.758518518516</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="19">
         <v>5</v>
@@ -7179,7 +7279,7 @@
         <v>4</v>
       </c>
       <c r="R16" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="S16" s="17"/>
       <c r="T16" s="17"/>
@@ -7193,10 +7293,10 @@
         <v>45607.774409722224</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D17" s="19">
         <v>4</v>
@@ -7241,7 +7341,7 @@
         <v>4</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="S17" s="17"/>
       <c r="T17" s="17"/>

</xml_diff>

<commit_message>
final update including Bella
</commit_message>
<xml_diff>
--- a/master_c4g_24.xlsx
+++ b/master_c4g_24.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jakefarren-price/Google Drive/RYA - Analysis/Crew4Gold_24/c4g/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DFF6599-7CFB-9548-A1E3-328DC3312B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1CE0EB5-D379-4C48-AD1F-5AF6A465B36B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10880" yWindow="-27680" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13380" yWindow="-28300" windowWidth="34400" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="overall" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="15" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="213">
   <si>
     <t>Name</t>
   </si>
@@ -679,6 +679,9 @@
   </si>
   <si>
     <t>Age</t>
+  </si>
+  <si>
+    <t>Bella Fellows (Helm)</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="175" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="11" x14ac:knownFonts="1">
     <font>
@@ -1078,7 +1081,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1165,8 +1168,7 @@
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1262,30 +1264,30 @@
     <xf numFmtId="10" fontId="9" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="175" fontId="10" fillId="30" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="31" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="44" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="45" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="46" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="47" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="175" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="30" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="31" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="32" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="33" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="34" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="35" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="36" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="37" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="38" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="39" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="40" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="41" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="42" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="43" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="44" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="45" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="46" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="47" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="20">
     <dxf>
       <alignment wrapText="1" indent="0"/>
     </dxf>
@@ -1338,67 +1340,7 @@
       <alignment wrapText="1" indent="0"/>
     </dxf>
     <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="175" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
-    </dxf>
-    <dxf>
-      <alignment wrapText="1" indent="0"/>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <alignment wrapText="1"/>
@@ -3887,7 +3829,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3200E97E-E608-2941-A9E2-A293371AF9A7}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{3200E97E-E608-2941-A9E2-A293371AF9A7}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:O16" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -4034,10 +3976,10 @@
     <dataField name="Average of Behaviours [Preparing and reviewing training]" fld="16" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="39">
+    <format dxfId="19">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="38">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="14">
@@ -4059,7 +4001,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="20">
+    <format dxfId="17">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
@@ -4104,7 +4046,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95A770F9-FC95-F442-B2CC-40B5FC752FC4}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{95A770F9-FC95-F442-B2CC-40B5FC752FC4}" name="PivotTable2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:A62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="18">
     <pivotField showAll="0"/>
@@ -4372,23 +4314,23 @@
     <i/>
   </colItems>
   <formats count="17">
-    <format dxfId="37">
+    <format dxfId="16">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="15">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="14">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="2" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="13">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="12">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4400,7 +4342,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4413,7 +4355,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4426,7 +4368,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="9">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4438,7 +4380,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="8">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4450,7 +4392,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4462,7 +4404,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="27">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4474,7 +4416,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="26">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4486,7 +4428,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="25">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4499,7 +4441,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="24">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4511,7 +4453,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="23">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4523,7 +4465,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="22">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4536,7 +4478,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="21">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="2" count="1" selected="0">
@@ -4853,13 +4795,13 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H39" sqref="H39"/>
+      <selection pane="topRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="15" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="15" style="9" customWidth="1"/>
     <col min="7" max="8" width="15" style="14" bestFit="1" customWidth="1"/>
@@ -5006,26 +4948,26 @@
       <c r="F2" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G2" s="65">
+      <c r="G2" s="64">
         <v>60</v>
       </c>
-      <c r="H2" s="65">
+      <c r="H2" s="64">
         <v>160</v>
       </c>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
       <c r="L2" s="9" t="s">
         <v>107</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N2" s="66">
+      <c r="N2" s="65">
         <v>0.01</v>
       </c>
       <c r="O2" s="9">
-        <f>_xlfn.RANK.AVG(N2,$N$2:$N$13)</f>
+        <f t="shared" ref="O2:O10" si="0">_xlfn.RANK.AVG(N2,$N$2:$N$13)</f>
         <v>12</v>
       </c>
       <c r="P2" s="10">
@@ -5036,46 +4978,46 @@
         <f>P2*G2/100</f>
         <v>55.68</v>
       </c>
-      <c r="R2" s="67">
-        <v>3</v>
-      </c>
-      <c r="S2" s="67">
-        <v>3</v>
-      </c>
-      <c r="T2" s="67">
-        <v>3</v>
-      </c>
-      <c r="U2" s="68">
-        <v>4</v>
-      </c>
-      <c r="V2" s="68">
-        <v>4</v>
-      </c>
-      <c r="W2" s="67">
-        <v>3</v>
-      </c>
-      <c r="X2" s="67">
-        <v>3</v>
-      </c>
-      <c r="Y2" s="68">
-        <v>4</v>
-      </c>
-      <c r="Z2" s="68">
-        <v>4</v>
-      </c>
-      <c r="AA2" s="68">
-        <v>4</v>
-      </c>
-      <c r="AB2" s="67">
-        <v>3</v>
-      </c>
-      <c r="AC2" s="69">
+      <c r="R2" s="66">
+        <v>3</v>
+      </c>
+      <c r="S2" s="66">
+        <v>3</v>
+      </c>
+      <c r="T2" s="66">
+        <v>3</v>
+      </c>
+      <c r="U2" s="67">
+        <v>4</v>
+      </c>
+      <c r="V2" s="67">
+        <v>4</v>
+      </c>
+      <c r="W2" s="66">
+        <v>3</v>
+      </c>
+      <c r="X2" s="66">
+        <v>3</v>
+      </c>
+      <c r="Y2" s="67">
+        <v>4</v>
+      </c>
+      <c r="Z2" s="67">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="67">
+        <v>4</v>
+      </c>
+      <c r="AB2" s="66">
+        <v>3</v>
+      </c>
+      <c r="AC2" s="68">
         <v>2</v>
       </c>
-      <c r="AD2" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE2" s="67">
+      <c r="AD2" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE2" s="66">
         <v>3</v>
       </c>
       <c r="AF2" s="26">
@@ -5087,11 +5029,11 @@
         <v>3.1666666666666665</v>
       </c>
       <c r="AH2" s="9">
-        <f t="shared" ref="AH2:AH13" si="0">_xlfn.RANK.AVG(AF2,$AF$2:$AF$13)</f>
+        <f t="shared" ref="AH2:AH13" si="1">_xlfn.RANK.AVG(AF2,$AF$2:$AF$13)</f>
         <v>6</v>
       </c>
       <c r="AI2" s="9">
-        <f t="shared" ref="AI2:AI13" si="1">_xlfn.RANK.AVG(AG2,$AG$2:$AG$13)</f>
+        <f t="shared" ref="AI2:AI13" si="2">_xlfn.RANK.AVG(AG2,$AG$2:$AG$13)</f>
         <v>12</v>
       </c>
       <c r="AJ2" t="s">
@@ -5117,19 +5059,19 @@
       <c r="F3" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G3" s="38">
+      <c r="G3" s="37">
         <v>71.5</v>
       </c>
-      <c r="H3" s="38">
+      <c r="H3" s="37">
         <v>173</v>
       </c>
-      <c r="I3" s="40">
+      <c r="I3" s="39">
         <v>4.5999999999999996</v>
       </c>
-      <c r="J3" s="40">
+      <c r="J3" s="39">
         <v>0.9</v>
       </c>
-      <c r="K3" s="40">
+      <c r="K3" s="39">
         <v>3.3</v>
       </c>
       <c r="L3" s="9" t="s">
@@ -5138,77 +5080,77 @@
       <c r="M3" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N3" s="42">
+      <c r="N3" s="41">
         <v>0.73</v>
       </c>
       <c r="O3" s="9">
-        <f>_xlfn.RANK.AVG(N3,$N$2:$N$13)</f>
-        <v>7</v>
-      </c>
-      <c r="P3" s="10">
-        <f t="shared" ref="P3:P8" si="2">0.58*H3</f>
-        <v>100.33999999999999</v>
-      </c>
-      <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q8" si="3">P3*G3/100</f>
-        <v>71.743099999999998</v>
-      </c>
-      <c r="R3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="S3" s="67">
-        <v>3</v>
-      </c>
-      <c r="T3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="U3" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="V3" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="W3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="X3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="Y3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="Z3" s="68">
-        <v>4</v>
-      </c>
-      <c r="AA3" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="AB3" s="73">
-        <v>4.3</v>
-      </c>
-      <c r="AC3" s="68">
-        <v>4</v>
-      </c>
-      <c r="AD3" s="73">
-        <v>4.3</v>
-      </c>
-      <c r="AE3" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="AF3" s="26">
-        <f t="shared" ref="AF3:AF13" si="4">AVERAGE(R3:Y3)</f>
-        <v>3.35</v>
-      </c>
-      <c r="AG3" s="26">
-        <f t="shared" ref="AG3:AG13" si="5">AVERAGE(Z3:AE3)</f>
-        <v>3.9499999999999997</v>
-      </c>
-      <c r="AH3" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
+      <c r="P3" s="10">
+        <f t="shared" ref="P3:P8" si="3">0.58*H3</f>
+        <v>100.33999999999999</v>
+      </c>
+      <c r="Q3" s="10">
+        <f t="shared" ref="Q3:Q8" si="4">P3*G3/100</f>
+        <v>71.743099999999998</v>
+      </c>
+      <c r="R3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="S3" s="66">
+        <v>3</v>
+      </c>
+      <c r="T3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="U3" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="V3" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="W3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="X3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="Y3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="Z3" s="67">
+        <v>4</v>
+      </c>
+      <c r="AA3" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="AB3" s="72">
+        <v>4.3</v>
+      </c>
+      <c r="AC3" s="67">
+        <v>4</v>
+      </c>
+      <c r="AD3" s="72">
+        <v>4.3</v>
+      </c>
+      <c r="AE3" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="AF3" s="26">
+        <f t="shared" ref="AF3:AF13" si="5">AVERAGE(R3:Y3)</f>
+        <v>3.35</v>
+      </c>
+      <c r="AG3" s="26">
+        <f t="shared" ref="AG3:AG13" si="6">AVERAGE(Z3:AE3)</f>
+        <v>3.9499999999999997</v>
+      </c>
+      <c r="AH3" s="9">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="AI3" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="AJ3" t="s">
@@ -5234,19 +5176,19 @@
       <c r="F4" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="37">
         <v>56.9</v>
       </c>
-      <c r="H4" s="38">
+      <c r="H4" s="37">
         <v>168</v>
       </c>
-      <c r="I4" s="40">
+      <c r="I4" s="39">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J4" s="40">
+      <c r="J4" s="39">
         <v>1</v>
       </c>
-      <c r="K4" s="40">
+      <c r="K4" s="39">
         <v>4</v>
       </c>
       <c r="L4" s="9" t="s">
@@ -5255,77 +5197,77 @@
       <c r="M4" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N4" s="42">
+      <c r="N4" s="41">
         <v>0.9</v>
       </c>
       <c r="O4" s="9">
-        <f>_xlfn.RANK.AVG(N4,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="P4" s="10">
+        <f t="shared" si="3"/>
+        <v>97.44</v>
+      </c>
+      <c r="Q4" s="10">
+        <f t="shared" si="4"/>
+        <v>55.443359999999991</v>
+      </c>
+      <c r="R4" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="S4" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="T4" s="66">
+        <v>3</v>
+      </c>
+      <c r="U4" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="V4" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="W4" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="X4" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="Y4" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="Z4" s="73">
+        <v>3.6</v>
+      </c>
+      <c r="AA4" s="67">
+        <v>4</v>
+      </c>
+      <c r="AB4" s="72">
+        <v>4.3</v>
+      </c>
+      <c r="AC4" s="67">
+        <v>4</v>
+      </c>
+      <c r="AD4" s="72">
+        <v>4.3</v>
+      </c>
+      <c r="AE4" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="AF4" s="26">
+        <f t="shared" si="5"/>
+        <v>3.5125000000000002</v>
+      </c>
+      <c r="AG4" s="26">
+        <f t="shared" si="6"/>
+        <v>4</v>
+      </c>
+      <c r="AH4" s="9">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="AI4" s="9">
         <f t="shared" si="2"/>
-        <v>97.44</v>
-      </c>
-      <c r="Q4" s="10">
-        <f t="shared" si="3"/>
-        <v>55.443359999999991</v>
-      </c>
-      <c r="R4" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="S4" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="T4" s="67">
-        <v>3</v>
-      </c>
-      <c r="U4" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="V4" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="W4" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="X4" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="Y4" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="Z4" s="74">
-        <v>3.6</v>
-      </c>
-      <c r="AA4" s="68">
-        <v>4</v>
-      </c>
-      <c r="AB4" s="73">
-        <v>4.3</v>
-      </c>
-      <c r="AC4" s="68">
-        <v>4</v>
-      </c>
-      <c r="AD4" s="73">
-        <v>4.3</v>
-      </c>
-      <c r="AE4" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="AF4" s="26">
-        <f t="shared" si="4"/>
-        <v>3.5125000000000002</v>
-      </c>
-      <c r="AG4" s="26">
-        <f t="shared" si="5"/>
-        <v>4</v>
-      </c>
-      <c r="AH4" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="AI4" s="9">
-        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AJ4" t="s">
@@ -5351,19 +5293,19 @@
       <c r="F5" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G5" s="38">
+      <c r="G5" s="37">
         <v>68.099999999999994</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="37">
         <v>167.1</v>
       </c>
-      <c r="I5" s="40">
+      <c r="I5" s="39">
         <v>3.7</v>
       </c>
-      <c r="J5" s="40">
+      <c r="J5" s="39">
         <v>1</v>
       </c>
-      <c r="K5" s="40">
+      <c r="K5" s="39">
         <v>3.7</v>
       </c>
       <c r="L5" s="9" t="s">
@@ -5372,77 +5314,77 @@
       <c r="M5" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N5" s="42">
+      <c r="N5" s="41">
         <v>0.8</v>
       </c>
       <c r="O5" s="9">
-        <f>_xlfn.RANK.AVG(N5,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="P5" s="10">
+        <f t="shared" si="3"/>
+        <v>96.917999999999992</v>
+      </c>
+      <c r="Q5" s="10">
+        <f t="shared" si="4"/>
+        <v>66.00115799999999</v>
+      </c>
+      <c r="R5" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="S5" s="67">
+        <v>4</v>
+      </c>
+      <c r="T5" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="U5" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="V5" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="W5" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="X5" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="Y5" s="66">
+        <v>3</v>
+      </c>
+      <c r="Z5" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AA5" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AB5" s="76">
+        <v>2.8</v>
+      </c>
+      <c r="AC5" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="AD5" s="69">
+        <v>3.3</v>
+      </c>
+      <c r="AE5" s="66">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="26">
+        <f t="shared" si="5"/>
+        <v>3.45</v>
+      </c>
+      <c r="AG5" s="26">
+        <f t="shared" si="6"/>
+        <v>3.3000000000000003</v>
+      </c>
+      <c r="AH5" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="AI5" s="9">
         <f t="shared" si="2"/>
-        <v>96.917999999999992</v>
-      </c>
-      <c r="Q5" s="10">
-        <f t="shared" si="3"/>
-        <v>66.00115799999999</v>
-      </c>
-      <c r="R5" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="S5" s="68">
-        <v>4</v>
-      </c>
-      <c r="T5" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="U5" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="V5" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="W5" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="X5" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="Y5" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z5" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AA5" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AB5" s="77">
-        <v>2.8</v>
-      </c>
-      <c r="AC5" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="AD5" s="70">
-        <v>3.3</v>
-      </c>
-      <c r="AE5" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF5" s="26">
-        <f t="shared" si="4"/>
-        <v>3.45</v>
-      </c>
-      <c r="AG5" s="26">
-        <f t="shared" si="5"/>
-        <v>3.3000000000000003</v>
-      </c>
-      <c r="AH5" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="AI5" s="9">
-        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="AJ5" t="s">
@@ -5468,19 +5410,19 @@
       <c r="F6" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G6" s="38">
+      <c r="G6" s="37">
         <v>70.3</v>
       </c>
-      <c r="H6" s="38">
+      <c r="H6" s="37">
         <v>168.5</v>
       </c>
-      <c r="I6" s="40">
+      <c r="I6" s="39">
         <v>4.0999999999999996</v>
       </c>
-      <c r="J6" s="40">
+      <c r="J6" s="39">
         <v>0.9</v>
       </c>
-      <c r="K6" s="40">
+      <c r="K6" s="39">
         <v>3.4</v>
       </c>
       <c r="L6" s="9" t="s">
@@ -5489,77 +5431,77 @@
       <c r="M6" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N6" s="42">
+      <c r="N6" s="41">
         <v>0.56000000000000005</v>
       </c>
       <c r="O6" s="9">
-        <f>_xlfn.RANK.AVG(N6,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="P6" s="10">
+        <f t="shared" si="3"/>
+        <v>97.72999999999999</v>
+      </c>
+      <c r="Q6" s="10">
+        <f t="shared" si="4"/>
+        <v>68.704189999999983</v>
+      </c>
+      <c r="R6" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="S6" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="T6" s="66">
+        <v>3</v>
+      </c>
+      <c r="U6" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="V6" s="66">
+        <v>3</v>
+      </c>
+      <c r="W6" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="X6" s="67">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="77">
+        <v>2.5</v>
+      </c>
+      <c r="Z6" s="66">
+        <v>3</v>
+      </c>
+      <c r="AA6" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="AB6" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AC6" s="66">
+        <v>3</v>
+      </c>
+      <c r="AD6" s="67">
+        <v>4</v>
+      </c>
+      <c r="AE6" s="67">
+        <v>4</v>
+      </c>
+      <c r="AF6" s="26">
+        <f t="shared" si="5"/>
+        <v>3.3125</v>
+      </c>
+      <c r="AG6" s="26">
+        <f t="shared" si="6"/>
+        <v>3.5</v>
+      </c>
+      <c r="AH6" s="9">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="AI6" s="9">
         <f t="shared" si="2"/>
-        <v>97.72999999999999</v>
-      </c>
-      <c r="Q6" s="10">
-        <f t="shared" si="3"/>
-        <v>68.704189999999983</v>
-      </c>
-      <c r="R6" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="S6" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="T6" s="67">
-        <v>3</v>
-      </c>
-      <c r="U6" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="V6" s="67">
-        <v>3</v>
-      </c>
-      <c r="W6" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="X6" s="68">
-        <v>4</v>
-      </c>
-      <c r="Y6" s="78">
-        <v>2.5</v>
-      </c>
-      <c r="Z6" s="67">
-        <v>3</v>
-      </c>
-      <c r="AA6" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="AB6" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AC6" s="67">
-        <v>3</v>
-      </c>
-      <c r="AD6" s="68">
-        <v>4</v>
-      </c>
-      <c r="AE6" s="68">
-        <v>4</v>
-      </c>
-      <c r="AF6" s="26">
-        <f t="shared" si="4"/>
-        <v>3.3125</v>
-      </c>
-      <c r="AG6" s="26">
-        <f t="shared" si="5"/>
-        <v>3.5</v>
-      </c>
-      <c r="AH6" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="AI6" s="9">
-        <f t="shared" si="1"/>
         <v>8.5</v>
       </c>
       <c r="AJ6" t="s">
@@ -5585,19 +5527,19 @@
       <c r="F7" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="37">
         <v>63.35</v>
       </c>
-      <c r="H7" s="38">
+      <c r="H7" s="37">
         <v>164.1</v>
       </c>
-      <c r="I7" s="40">
+      <c r="I7" s="39">
         <v>0</v>
       </c>
-      <c r="J7" s="40">
+      <c r="J7" s="39">
         <v>0.8</v>
       </c>
-      <c r="K7" s="40">
+      <c r="K7" s="39">
         <v>4.0999999999999996</v>
       </c>
       <c r="L7" s="9" t="s">
@@ -5606,77 +5548,77 @@
       <c r="M7" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N7" s="42">
+      <c r="N7" s="41">
         <v>0.79</v>
       </c>
       <c r="O7" s="9">
-        <f>_xlfn.RANK.AVG(N7,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="P7" s="10">
+        <f t="shared" si="3"/>
+        <v>95.177999999999983</v>
+      </c>
+      <c r="Q7" s="10">
+        <f t="shared" si="4"/>
+        <v>60.295262999999984</v>
+      </c>
+      <c r="R7" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="S7" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="T7" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="U7" s="67">
+        <v>4</v>
+      </c>
+      <c r="V7" s="67">
+        <v>4</v>
+      </c>
+      <c r="W7" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="X7" s="67">
+        <v>4</v>
+      </c>
+      <c r="Y7" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="Z7" s="67">
+        <v>4</v>
+      </c>
+      <c r="AA7" s="78">
+        <v>4.5</v>
+      </c>
+      <c r="AB7" s="67">
+        <v>4</v>
+      </c>
+      <c r="AC7" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AD7" s="79">
+        <v>4.7</v>
+      </c>
+      <c r="AE7" s="67">
+        <v>4</v>
+      </c>
+      <c r="AF7" s="26">
+        <f t="shared" si="5"/>
+        <v>3.6875</v>
+      </c>
+      <c r="AG7" s="26">
+        <f t="shared" si="6"/>
+        <v>4.1499999999999995</v>
+      </c>
+      <c r="AH7" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="AI7" s="9">
         <f t="shared" si="2"/>
-        <v>95.177999999999983</v>
-      </c>
-      <c r="Q7" s="10">
-        <f t="shared" si="3"/>
-        <v>60.295262999999984</v>
-      </c>
-      <c r="R7" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="S7" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="T7" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="U7" s="68">
-        <v>4</v>
-      </c>
-      <c r="V7" s="68">
-        <v>4</v>
-      </c>
-      <c r="W7" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="X7" s="68">
-        <v>4</v>
-      </c>
-      <c r="Y7" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="Z7" s="68">
-        <v>4</v>
-      </c>
-      <c r="AA7" s="79">
-        <v>4.5</v>
-      </c>
-      <c r="AB7" s="68">
-        <v>4</v>
-      </c>
-      <c r="AC7" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AD7" s="80">
-        <v>4.7</v>
-      </c>
-      <c r="AE7" s="68">
-        <v>4</v>
-      </c>
-      <c r="AF7" s="26">
-        <f t="shared" si="4"/>
-        <v>3.6875</v>
-      </c>
-      <c r="AG7" s="26">
-        <f t="shared" si="5"/>
-        <v>4.1499999999999995</v>
-      </c>
-      <c r="AH7" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="AI7" s="9">
-        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="AJ7" t="s">
@@ -5702,19 +5644,19 @@
       <c r="F8" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="38">
+      <c r="G8" s="37">
         <v>62.35</v>
       </c>
-      <c r="H8" s="38">
+      <c r="H8" s="37">
         <v>168.3</v>
       </c>
-      <c r="I8" s="40">
+      <c r="I8" s="39">
         <v>0</v>
       </c>
-      <c r="J8" s="40">
+      <c r="J8" s="39">
         <v>0.7</v>
       </c>
-      <c r="K8" s="40">
+      <c r="K8" s="39">
         <v>3.4</v>
       </c>
       <c r="L8" s="9" t="s">
@@ -5723,77 +5665,77 @@
       <c r="M8" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="N8" s="42">
+      <c r="N8" s="41">
         <v>0.7</v>
       </c>
       <c r="O8" s="9">
-        <f>_xlfn.RANK.AVG(N8,$N$2:$N$13)</f>
-        <v>9</v>
-      </c>
-      <c r="P8" s="10">
-        <f t="shared" si="2"/>
-        <v>97.614000000000004</v>
-      </c>
-      <c r="Q8" s="10">
-        <f t="shared" si="3"/>
-        <v>60.862329000000003</v>
-      </c>
-      <c r="R8" s="68">
-        <v>4</v>
-      </c>
-      <c r="S8" s="67">
-        <v>3</v>
-      </c>
-      <c r="T8" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="U8" s="78">
-        <v>2.5</v>
-      </c>
-      <c r="V8" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="W8" s="67">
-        <v>3</v>
-      </c>
-      <c r="X8" s="67">
-        <v>3</v>
-      </c>
-      <c r="Y8" s="67">
-        <v>3</v>
-      </c>
-      <c r="Z8" s="81">
-        <v>4.3</v>
-      </c>
-      <c r="AA8" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AB8" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AC8" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AD8" s="68">
-        <v>4</v>
-      </c>
-      <c r="AE8" s="67">
-        <v>3</v>
-      </c>
-      <c r="AF8" s="26">
-        <f t="shared" si="4"/>
-        <v>3.1875</v>
-      </c>
-      <c r="AG8" s="26">
-        <f t="shared" si="5"/>
-        <v>3.7333333333333329</v>
-      </c>
-      <c r="AH8" s="9">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
+      <c r="P8" s="10">
+        <f t="shared" si="3"/>
+        <v>97.614000000000004</v>
+      </c>
+      <c r="Q8" s="10">
+        <f t="shared" si="4"/>
+        <v>60.862329000000003</v>
+      </c>
+      <c r="R8" s="67">
+        <v>4</v>
+      </c>
+      <c r="S8" s="66">
+        <v>3</v>
+      </c>
+      <c r="T8" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="U8" s="77">
+        <v>2.5</v>
+      </c>
+      <c r="V8" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="W8" s="66">
+        <v>3</v>
+      </c>
+      <c r="X8" s="66">
+        <v>3</v>
+      </c>
+      <c r="Y8" s="66">
+        <v>3</v>
+      </c>
+      <c r="Z8" s="80">
+        <v>4.3</v>
+      </c>
+      <c r="AA8" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AB8" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AC8" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AD8" s="67">
+        <v>4</v>
+      </c>
+      <c r="AE8" s="66">
+        <v>3</v>
+      </c>
+      <c r="AF8" s="26">
+        <f t="shared" si="5"/>
+        <v>3.1875</v>
+      </c>
+      <c r="AG8" s="26">
+        <f t="shared" si="6"/>
+        <v>3.7333333333333329</v>
+      </c>
+      <c r="AH8" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
       <c r="AI8" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="AJ8" t="s">
@@ -5819,19 +5761,19 @@
       <c r="F9" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G9" s="38">
+      <c r="G9" s="37">
         <v>72.05</v>
       </c>
-      <c r="H9" s="38">
+      <c r="H9" s="37">
         <v>176.6</v>
       </c>
-      <c r="I9" s="40">
-        <v>4</v>
-      </c>
-      <c r="J9" s="40">
+      <c r="I9" s="39">
+        <v>4</v>
+      </c>
+      <c r="J9" s="39">
         <v>0.8</v>
       </c>
-      <c r="K9" s="40">
+      <c r="K9" s="39">
         <v>3.4</v>
       </c>
       <c r="L9" s="9" t="s">
@@ -5840,11 +5782,11 @@
       <c r="M9" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="N9" s="42">
+      <c r="N9" s="41">
         <v>0.65</v>
       </c>
       <c r="O9" s="9">
-        <f>_xlfn.RANK.AVG(N9,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="P9" s="10">
@@ -5855,62 +5797,62 @@
         <f>P9*G9/100</f>
         <v>73.799373999999986</v>
       </c>
-      <c r="R9" s="67">
-        <v>3</v>
-      </c>
-      <c r="S9" s="78">
+      <c r="R9" s="66">
+        <v>3</v>
+      </c>
+      <c r="S9" s="77">
         <v>2.5</v>
       </c>
-      <c r="T9" s="67">
-        <v>3</v>
-      </c>
-      <c r="U9" s="72">
+      <c r="T9" s="66">
+        <v>3</v>
+      </c>
+      <c r="U9" s="71">
         <v>3.5</v>
       </c>
-      <c r="V9" s="67">
-        <v>3</v>
-      </c>
-      <c r="W9" s="78">
+      <c r="V9" s="66">
+        <v>3</v>
+      </c>
+      <c r="W9" s="77">
         <v>2.5</v>
       </c>
-      <c r="X9" s="67">
-        <v>3</v>
-      </c>
-      <c r="Y9" s="78">
+      <c r="X9" s="66">
+        <v>3</v>
+      </c>
+      <c r="Y9" s="77">
         <v>2.5</v>
       </c>
-      <c r="Z9" s="75">
+      <c r="Z9" s="74">
         <v>3.3</v>
       </c>
-      <c r="AA9" s="67">
-        <v>3</v>
-      </c>
-      <c r="AB9" s="76">
+      <c r="AA9" s="66">
+        <v>3</v>
+      </c>
+      <c r="AB9" s="75">
         <v>3.7</v>
       </c>
-      <c r="AC9" s="75">
+      <c r="AC9" s="74">
         <v>3.3</v>
       </c>
-      <c r="AD9" s="68">
-        <v>4</v>
-      </c>
-      <c r="AE9" s="76">
+      <c r="AD9" s="67">
+        <v>4</v>
+      </c>
+      <c r="AE9" s="75">
         <v>3.7</v>
       </c>
       <c r="AF9" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.875</v>
       </c>
       <c r="AG9" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.5</v>
       </c>
       <c r="AH9" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="AI9" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
       <c r="AJ9" t="s">
@@ -5957,11 +5899,11 @@
       <c r="M10" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N10" s="43">
+      <c r="N10" s="42">
         <v>0.79</v>
       </c>
       <c r="O10" s="9">
-        <f>_xlfn.RANK.AVG(N10,$N$2:$N$13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="P10" s="10">
@@ -5972,62 +5914,62 @@
         <f>P10*G10/100</f>
         <v>59.548832000000004</v>
       </c>
-      <c r="R10" s="76">
+      <c r="R10" s="75">
         <v>3.7</v>
       </c>
-      <c r="S10" s="68">
-        <v>4</v>
-      </c>
-      <c r="T10" s="67">
-        <v>3</v>
-      </c>
-      <c r="U10" s="67">
-        <v>3</v>
-      </c>
-      <c r="V10" s="76">
+      <c r="S10" s="67">
+        <v>4</v>
+      </c>
+      <c r="T10" s="66">
+        <v>3</v>
+      </c>
+      <c r="U10" s="66">
+        <v>3</v>
+      </c>
+      <c r="V10" s="75">
         <v>3.7</v>
       </c>
-      <c r="W10" s="76">
+      <c r="W10" s="75">
         <v>3.7</v>
       </c>
-      <c r="X10" s="76">
+      <c r="X10" s="75">
         <v>3.7</v>
       </c>
-      <c r="Y10" s="75">
+      <c r="Y10" s="74">
         <v>3.3</v>
       </c>
-      <c r="Z10" s="71">
+      <c r="Z10" s="70">
         <v>3.8</v>
       </c>
-      <c r="AA10" s="67">
-        <v>3</v>
-      </c>
-      <c r="AB10" s="67">
-        <v>3</v>
-      </c>
-      <c r="AC10" s="68">
-        <v>4</v>
-      </c>
-      <c r="AD10" s="67">
-        <v>3</v>
-      </c>
-      <c r="AE10" s="72">
+      <c r="AA10" s="66">
+        <v>3</v>
+      </c>
+      <c r="AB10" s="66">
+        <v>3</v>
+      </c>
+      <c r="AC10" s="67">
+        <v>4</v>
+      </c>
+      <c r="AD10" s="66">
+        <v>3</v>
+      </c>
+      <c r="AE10" s="71">
         <v>3.5</v>
       </c>
       <c r="AF10" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.5124999999999997</v>
       </c>
       <c r="AG10" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.3833333333333333</v>
       </c>
       <c r="AH10" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="AI10" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="AJ10" t="s">
@@ -6059,13 +6001,13 @@
       <c r="H11" s="29">
         <v>173.4</v>
       </c>
-      <c r="I11" s="40">
+      <c r="I11" s="39">
         <v>3.8</v>
       </c>
-      <c r="J11" s="40">
+      <c r="J11" s="39">
         <v>0.7</v>
       </c>
-      <c r="K11" s="40">
+      <c r="K11" s="39">
         <v>3.2</v>
       </c>
       <c r="L11" s="9" t="s">
@@ -6074,77 +6016,77 @@
       <c r="M11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="N11" s="43">
+      <c r="N11" s="42">
         <v>0.79</v>
       </c>
       <c r="O11" s="9">
-        <f t="shared" ref="O11:O12" si="6">_xlfn.RANK.AVG(N11,$N$2:$N$13)</f>
+        <f t="shared" ref="O11:O12" si="7">_xlfn.RANK.AVG(N11,$N$2:$N$13)</f>
         <v>5</v>
       </c>
       <c r="P11" s="10">
-        <f t="shared" ref="P11:P12" si="7">0.58*H11</f>
+        <f t="shared" ref="P11:P12" si="8">0.58*H11</f>
         <v>100.572</v>
       </c>
       <c r="Q11" s="10">
-        <f t="shared" ref="Q11:Q13" si="8">P11*G11/100</f>
+        <f t="shared" ref="Q11:Q14" si="9">P11*G11/100</f>
         <v>75.831288000000001</v>
       </c>
-      <c r="R11" s="82">
+      <c r="R11" s="81">
         <v>1.7</v>
       </c>
-      <c r="S11" s="69">
+      <c r="S11" s="68">
         <v>2</v>
       </c>
-      <c r="T11" s="83">
+      <c r="T11" s="82">
         <v>2.2999999999999998</v>
       </c>
-      <c r="U11" s="84">
+      <c r="U11" s="83">
         <v>2.7</v>
       </c>
-      <c r="V11" s="84">
+      <c r="V11" s="83">
         <v>2.7</v>
       </c>
-      <c r="W11" s="84">
+      <c r="W11" s="83">
         <v>2.7</v>
       </c>
-      <c r="X11" s="84">
+      <c r="X11" s="83">
         <v>2.7</v>
       </c>
-      <c r="Y11" s="84">
+      <c r="Y11" s="83">
         <v>2.7</v>
       </c>
-      <c r="Z11" s="67">
-        <v>3</v>
-      </c>
-      <c r="AA11" s="84">
+      <c r="Z11" s="66">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="83">
         <v>2.7</v>
       </c>
-      <c r="AB11" s="79">
+      <c r="AB11" s="78">
         <v>4.5</v>
       </c>
-      <c r="AC11" s="68">
-        <v>4</v>
-      </c>
-      <c r="AD11" s="79">
+      <c r="AC11" s="67">
+        <v>4</v>
+      </c>
+      <c r="AD11" s="78">
         <v>4.5</v>
       </c>
-      <c r="AE11" s="85">
+      <c r="AE11" s="84">
         <v>4.8</v>
       </c>
       <c r="AF11" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.4374999999999996</v>
       </c>
       <c r="AG11" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9166666666666665</v>
       </c>
       <c r="AH11" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="AI11" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="AJ11" t="s">
@@ -6170,19 +6112,19 @@
       <c r="F12" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="37">
         <v>68.95</v>
       </c>
-      <c r="H12" s="38">
+      <c r="H12" s="37">
         <v>170.8</v>
       </c>
-      <c r="I12" s="41">
+      <c r="I12" s="40">
         <v>4.5</v>
       </c>
-      <c r="J12" s="41">
+      <c r="J12" s="40">
         <v>0.9</v>
       </c>
-      <c r="K12" s="41">
+      <c r="K12" s="40">
         <v>3.6</v>
       </c>
       <c r="L12" s="9" t="s">
@@ -6191,77 +6133,77 @@
       <c r="M12" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="N12" s="42">
+      <c r="N12" s="41">
         <v>0.91</v>
       </c>
       <c r="O12" s="9">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P12" s="10">
+        <f t="shared" si="8"/>
+        <v>99.063999999999993</v>
+      </c>
+      <c r="Q12" s="10">
+        <f t="shared" si="9"/>
+        <v>68.304628000000008</v>
+      </c>
+      <c r="R12" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="S12" s="83">
+        <v>2.7</v>
+      </c>
+      <c r="T12" s="83">
+        <v>2.7</v>
+      </c>
+      <c r="U12" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="V12" s="74">
+        <v>3.3</v>
+      </c>
+      <c r="W12" s="83">
+        <v>2.7</v>
+      </c>
+      <c r="X12" s="66">
+        <v>3</v>
+      </c>
+      <c r="Y12" s="83">
+        <v>2.7</v>
+      </c>
+      <c r="Z12" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="AA12" s="75">
+        <v>3.7</v>
+      </c>
+      <c r="AB12" s="71">
+        <v>3.5</v>
+      </c>
+      <c r="AC12" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="AD12" s="70">
+        <v>3.8</v>
+      </c>
+      <c r="AE12" s="67">
+        <v>4</v>
+      </c>
+      <c r="AF12" s="26">
+        <f t="shared" si="5"/>
+        <v>2.9624999999999999</v>
+      </c>
+      <c r="AG12" s="26">
         <f t="shared" si="6"/>
-        <v>1</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" si="7"/>
-        <v>99.063999999999993</v>
-      </c>
-      <c r="Q12" s="10">
-        <f t="shared" si="8"/>
-        <v>68.304628000000008</v>
-      </c>
-      <c r="R12" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="S12" s="84">
-        <v>2.7</v>
-      </c>
-      <c r="T12" s="84">
-        <v>2.7</v>
-      </c>
-      <c r="U12" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="V12" s="75">
-        <v>3.3</v>
-      </c>
-      <c r="W12" s="84">
-        <v>2.7</v>
-      </c>
-      <c r="X12" s="67">
-        <v>3</v>
-      </c>
-      <c r="Y12" s="84">
-        <v>2.7</v>
-      </c>
-      <c r="Z12" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="AA12" s="76">
-        <v>3.7</v>
-      </c>
-      <c r="AB12" s="72">
-        <v>3.5</v>
-      </c>
-      <c r="AC12" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="AD12" s="71">
-        <v>3.8</v>
-      </c>
-      <c r="AE12" s="68">
-        <v>4</v>
-      </c>
-      <c r="AF12" s="26">
-        <f t="shared" si="4"/>
-        <v>2.9624999999999999</v>
-      </c>
-      <c r="AG12" s="26">
-        <f t="shared" si="5"/>
         <v>3.7666666666666671</v>
       </c>
       <c r="AH12" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="AI12" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="AJ12" t="s">
@@ -6287,19 +6229,19 @@
       <c r="F13" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G13" s="38">
+      <c r="G13" s="37">
         <v>71.3</v>
       </c>
-      <c r="H13" s="38">
+      <c r="H13" s="37">
         <v>173</v>
       </c>
-      <c r="I13" s="41">
+      <c r="I13" s="40">
         <v>3.5</v>
       </c>
-      <c r="J13" s="41">
+      <c r="J13" s="40">
         <v>0.8</v>
       </c>
-      <c r="K13" s="41">
+      <c r="K13" s="40">
         <v>3.6</v>
       </c>
       <c r="L13" s="9" t="s">
@@ -6308,7 +6250,7 @@
       <c r="M13" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="N13" s="42">
+      <c r="N13" s="41">
         <v>0.72</v>
       </c>
       <c r="O13" s="9">
@@ -6320,69 +6262,94 @@
         <v>100.33999999999999</v>
       </c>
       <c r="Q13" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>71.542419999999993</v>
       </c>
-      <c r="R13" s="76">
+      <c r="R13" s="75">
         <v>3.7</v>
       </c>
-      <c r="S13" s="68">
-        <v>4</v>
-      </c>
-      <c r="T13" s="72">
+      <c r="S13" s="67">
+        <v>4</v>
+      </c>
+      <c r="T13" s="71">
         <v>3.5</v>
       </c>
-      <c r="U13" s="70">
+      <c r="U13" s="69">
         <v>3.3</v>
       </c>
-      <c r="V13" s="71">
+      <c r="V13" s="70">
         <v>3.8</v>
       </c>
-      <c r="W13" s="68">
-        <v>4</v>
-      </c>
-      <c r="X13" s="72">
+      <c r="W13" s="67">
+        <v>4</v>
+      </c>
+      <c r="X13" s="71">
         <v>3.5</v>
       </c>
-      <c r="Y13" s="70">
+      <c r="Y13" s="69">
         <v>3.3</v>
       </c>
-      <c r="Z13" s="72">
+      <c r="Z13" s="71">
         <v>3.5</v>
       </c>
-      <c r="AA13" s="68">
-        <v>4</v>
-      </c>
-      <c r="AB13" s="73">
+      <c r="AA13" s="67">
+        <v>4</v>
+      </c>
+      <c r="AB13" s="72">
         <v>4.3</v>
       </c>
-      <c r="AC13" s="71">
+      <c r="AC13" s="70">
         <v>3.8</v>
       </c>
-      <c r="AD13" s="79">
+      <c r="AD13" s="78">
         <v>4.5</v>
       </c>
-      <c r="AE13" s="71">
+      <c r="AE13" s="70">
         <v>3.8</v>
       </c>
       <c r="AF13" s="26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6375000000000002</v>
       </c>
       <c r="AG13" s="26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.9833333333333338</v>
       </c>
       <c r="AH13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="AI13" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="AJ13" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="14" spans="1:36" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="14">
+        <v>67</v>
+      </c>
+      <c r="H14" s="14">
+        <v>165</v>
+      </c>
+      <c r="P14" s="15">
+        <f>0.58*H14</f>
+        <v>95.699999999999989</v>
+      </c>
+      <c r="Q14" s="15">
+        <f t="shared" si="9"/>
+        <v>64.119</v>
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.2">
@@ -6606,310 +6573,310 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="3" spans="2:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="33" t="s">
         <v>161</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="33" t="s">
         <v>162</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="34" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="35" t="s">
+      <c r="E3" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="34" t="s">
+      <c r="G3" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="34" t="s">
+      <c r="H3" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="34" t="s">
+      <c r="I3" s="33" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="2:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="34" t="s">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="E4" s="34" t="s">
+      <c r="E4" s="33" t="s">
         <v>165</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="G4" s="34" t="s">
+      <c r="G4" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="H4" s="34" t="s">
+      <c r="H4" s="33" t="s">
         <v>167</v>
       </c>
-      <c r="I4" s="34" t="s">
+      <c r="I4" s="33" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="C5" s="37" t="s">
+      <c r="C5" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="D5" s="38">
+      <c r="D5" s="37">
         <v>71.5</v>
       </c>
-      <c r="E5" s="38">
+      <c r="E5" s="37">
         <v>173</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F5" s="43">
         <v>0.73</v>
       </c>
-      <c r="G5" s="45">
+      <c r="G5" s="44">
         <v>4.5999999999999996</v>
       </c>
-      <c r="H5" s="46">
+      <c r="H5" s="45">
         <v>0.9</v>
       </c>
-      <c r="I5" s="47">
+      <c r="I5" s="46">
         <v>3.3</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="36" t="s">
         <v>173</v>
       </c>
-      <c r="C6" s="37" t="s">
+      <c r="C6" s="36" t="s">
         <v>174</v>
       </c>
-      <c r="D6" s="38">
+      <c r="D6" s="37">
         <v>56.9</v>
       </c>
-      <c r="E6" s="38">
+      <c r="E6" s="37">
         <v>168</v>
       </c>
-      <c r="F6" s="48">
+      <c r="F6" s="47">
         <v>0.9</v>
       </c>
-      <c r="G6" s="49">
+      <c r="G6" s="48">
         <v>4.4000000000000004</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="44">
         <v>1</v>
       </c>
-      <c r="I6" s="50">
+      <c r="I6" s="49">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="C7" s="37" t="s">
+      <c r="C7" s="36" t="s">
         <v>180</v>
       </c>
-      <c r="D7" s="38">
+      <c r="D7" s="37">
         <v>68.099999999999994</v>
       </c>
-      <c r="E7" s="38">
+      <c r="E7" s="37">
         <v>167.1</v>
       </c>
-      <c r="F7" s="51">
+      <c r="F7" s="50">
         <v>0.8</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="51">
         <v>3.7</v>
       </c>
-      <c r="H7" s="45">
+      <c r="H7" s="44">
         <v>1</v>
       </c>
-      <c r="I7" s="53">
+      <c r="I7" s="52">
         <v>3.7</v>
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="36" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="38">
+      <c r="D8" s="37">
         <v>70.3</v>
       </c>
-      <c r="E8" s="38">
+      <c r="E8" s="37">
         <v>168.5</v>
       </c>
-      <c r="F8" s="47">
+      <c r="F8" s="46">
         <v>0.56000000000000005</v>
       </c>
-      <c r="G8" s="54">
+      <c r="G8" s="53">
         <v>4.0999999999999996</v>
       </c>
-      <c r="H8" s="46">
+      <c r="H8" s="45">
         <v>0.9</v>
       </c>
-      <c r="I8" s="55">
+      <c r="I8" s="54">
         <v>3.4</v>
       </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="36" t="s">
         <v>181</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C9" s="36" t="s">
         <v>182</v>
       </c>
-      <c r="D9" s="38">
+      <c r="D9" s="37">
         <v>63.35</v>
       </c>
-      <c r="E9" s="38">
+      <c r="E9" s="37">
         <v>164.1</v>
       </c>
-      <c r="F9" s="56">
+      <c r="F9" s="55">
         <v>0.79</v>
       </c>
-      <c r="G9" s="47">
+      <c r="G9" s="46">
         <v>0</v>
       </c>
-      <c r="H9" s="57">
+      <c r="H9" s="56">
         <v>0.8</v>
       </c>
-      <c r="I9" s="45">
+      <c r="I9" s="44">
         <v>4.0999999999999996</v>
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>177</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>178</v>
       </c>
-      <c r="D10" s="38">
+      <c r="D10" s="37">
         <v>62.35</v>
       </c>
-      <c r="E10" s="38">
+      <c r="E10" s="37">
         <v>168.3</v>
       </c>
-      <c r="F10" s="58">
+      <c r="F10" s="57">
         <v>0.7</v>
       </c>
-      <c r="G10" s="47">
+      <c r="G10" s="46">
         <v>0</v>
       </c>
-      <c r="H10" s="47">
+      <c r="H10" s="46">
         <v>0.7</v>
       </c>
-      <c r="I10" s="55">
+      <c r="I10" s="54">
         <v>3.4</v>
       </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
         <v>169</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>170</v>
       </c>
-      <c r="D11" s="38">
+      <c r="D11" s="37">
         <v>72.05</v>
       </c>
-      <c r="E11" s="38">
+      <c r="E11" s="37">
         <v>176.6</v>
       </c>
-      <c r="F11" s="59">
+      <c r="F11" s="58">
         <v>0.65</v>
       </c>
-      <c r="G11" s="60">
-        <v>4</v>
-      </c>
-      <c r="H11" s="57">
+      <c r="G11" s="59">
+        <v>4</v>
+      </c>
+      <c r="H11" s="56">
         <v>0.8</v>
       </c>
-      <c r="I11" s="55">
+      <c r="I11" s="54">
         <v>3.4</v>
       </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>172</v>
       </c>
-      <c r="D12" s="38">
+      <c r="D12" s="37">
         <v>68.95</v>
       </c>
-      <c r="E12" s="38">
+      <c r="E12" s="37">
         <v>170.8</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="44">
         <v>0.91</v>
       </c>
-      <c r="G12" s="61">
+      <c r="G12" s="60">
         <v>4.5</v>
       </c>
-      <c r="H12" s="46">
+      <c r="H12" s="45">
         <v>0.9</v>
       </c>
-      <c r="I12" s="62">
+      <c r="I12" s="61">
         <v>3.6</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="36" t="s">
         <v>171</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>176</v>
       </c>
-      <c r="D13" s="38">
+      <c r="D13" s="37">
         <v>71.3</v>
       </c>
-      <c r="E13" s="38">
+      <c r="E13" s="37">
         <v>173</v>
       </c>
-      <c r="F13" s="63">
+      <c r="F13" s="62">
         <v>0.72</v>
       </c>
-      <c r="G13" s="64">
+      <c r="G13" s="63">
         <v>3.5</v>
       </c>
-      <c r="H13" s="57">
+      <c r="H13" s="56">
         <v>0.8</v>
       </c>
-      <c r="I13" s="62">
+      <c r="I13" s="61">
         <v>3.6</v>
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="36" t="s">
         <v>186</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="36" t="s">
         <v>187</v>
       </c>
-      <c r="D14" s="38">
+      <c r="D14" s="37">
         <v>75.400000000000006</v>
       </c>
-      <c r="E14" s="38">
+      <c r="E14" s="37">
         <v>173.4</v>
       </c>
-      <c r="F14" s="39">
+      <c r="F14" s="38">
         <v>0.79</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="38">
         <v>3.8</v>
       </c>
-      <c r="H14" s="39">
+      <c r="H14" s="38">
         <v>0.7</v>
       </c>
-      <c r="I14" s="39">
+      <c r="I14" s="38">
         <v>3.2</v>
       </c>
     </row>
@@ -6994,46 +6961,46 @@
       <c r="A4" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="B4" s="33">
-        <v>3</v>
-      </c>
-      <c r="C4" s="33">
-        <v>3</v>
-      </c>
-      <c r="D4" s="33">
-        <v>3</v>
-      </c>
-      <c r="E4" s="33">
-        <v>4</v>
-      </c>
-      <c r="F4" s="33">
-        <v>4</v>
-      </c>
-      <c r="G4" s="33">
-        <v>3</v>
-      </c>
-      <c r="H4" s="33">
-        <v>3</v>
-      </c>
-      <c r="I4" s="33">
-        <v>4</v>
-      </c>
-      <c r="J4" s="33">
-        <v>4</v>
-      </c>
-      <c r="K4" s="33">
-        <v>4</v>
-      </c>
-      <c r="L4" s="33">
-        <v>3</v>
-      </c>
-      <c r="M4" s="33">
+      <c r="B4" s="32">
+        <v>3</v>
+      </c>
+      <c r="C4" s="32">
+        <v>3</v>
+      </c>
+      <c r="D4" s="32">
+        <v>3</v>
+      </c>
+      <c r="E4" s="32">
+        <v>4</v>
+      </c>
+      <c r="F4" s="32">
+        <v>4</v>
+      </c>
+      <c r="G4" s="32">
+        <v>3</v>
+      </c>
+      <c r="H4" s="32">
+        <v>3</v>
+      </c>
+      <c r="I4" s="32">
+        <v>4</v>
+      </c>
+      <c r="J4" s="32">
+        <v>4</v>
+      </c>
+      <c r="K4" s="32">
+        <v>4</v>
+      </c>
+      <c r="L4" s="32">
+        <v>3</v>
+      </c>
+      <c r="M4" s="32">
         <v>2</v>
       </c>
-      <c r="N4" s="33">
-        <v>3</v>
-      </c>
-      <c r="O4" s="33">
+      <c r="N4" s="32">
+        <v>3</v>
+      </c>
+      <c r="O4" s="32">
         <v>3</v>
       </c>
     </row>
@@ -7041,46 +7008,46 @@
       <c r="A5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="33">
+      <c r="B5" s="32">
         <v>3.25</v>
       </c>
-      <c r="C5" s="33">
-        <v>3</v>
-      </c>
-      <c r="D5" s="33">
+      <c r="C5" s="32">
+        <v>3</v>
+      </c>
+      <c r="D5" s="32">
         <v>3.25</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="32">
         <v>3.75</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>3.5</v>
       </c>
-      <c r="G5" s="33">
+      <c r="G5" s="32">
         <v>3.25</v>
       </c>
-      <c r="H5" s="33">
+      <c r="H5" s="32">
         <v>3.25</v>
       </c>
-      <c r="I5" s="33">
+      <c r="I5" s="32">
         <v>3.25</v>
       </c>
-      <c r="J5" s="33">
-        <v>4</v>
-      </c>
-      <c r="K5" s="33">
+      <c r="J5" s="32">
+        <v>4</v>
+      </c>
+      <c r="K5" s="32">
         <v>3.25</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="32">
         <v>4.25</v>
       </c>
-      <c r="M5" s="33">
-        <v>4</v>
-      </c>
-      <c r="N5" s="33">
+      <c r="M5" s="32">
+        <v>4</v>
+      </c>
+      <c r="N5" s="32">
         <v>4.25</v>
       </c>
-      <c r="O5" s="33">
+      <c r="O5" s="32">
         <v>3.75</v>
       </c>
     </row>
@@ -7088,46 +7055,46 @@
       <c r="A6" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B6" s="33">
+      <c r="B6" s="32">
         <v>3.5</v>
       </c>
-      <c r="C6" s="33">
+      <c r="C6" s="32">
         <v>3.5</v>
       </c>
-      <c r="D6" s="33">
-        <v>3</v>
-      </c>
-      <c r="E6" s="33">
+      <c r="D6" s="32">
+        <v>3</v>
+      </c>
+      <c r="E6" s="32">
         <v>3.75</v>
       </c>
-      <c r="F6" s="33">
+      <c r="F6" s="32">
         <v>3.5</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="32">
         <v>3.5</v>
       </c>
-      <c r="H6" s="33">
+      <c r="H6" s="32">
         <v>3.5</v>
       </c>
-      <c r="I6" s="33">
+      <c r="I6" s="32">
         <v>3.75</v>
       </c>
-      <c r="J6" s="33">
+      <c r="J6" s="32">
         <v>3.6</v>
       </c>
-      <c r="K6" s="33">
-        <v>4</v>
-      </c>
-      <c r="L6" s="33">
+      <c r="K6" s="32">
+        <v>4</v>
+      </c>
+      <c r="L6" s="32">
         <v>4.25</v>
       </c>
-      <c r="M6" s="33">
-        <v>4</v>
-      </c>
-      <c r="N6" s="33">
+      <c r="M6" s="32">
+        <v>4</v>
+      </c>
+      <c r="N6" s="32">
         <v>4.25</v>
       </c>
-      <c r="O6" s="33">
+      <c r="O6" s="32">
         <v>3.75</v>
       </c>
     </row>
@@ -7135,46 +7102,46 @@
       <c r="A7" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="33">
+      <c r="B7" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="C7" s="33">
-        <v>4</v>
-      </c>
-      <c r="D7" s="33">
+      <c r="C7" s="32">
+        <v>4</v>
+      </c>
+      <c r="D7" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F7" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="H7" s="33">
+      <c r="H7" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="I7" s="33">
-        <v>3</v>
-      </c>
-      <c r="J7" s="33">
+      <c r="I7" s="32">
+        <v>3</v>
+      </c>
+      <c r="J7" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="K7" s="33">
+      <c r="K7" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="L7" s="33">
+      <c r="L7" s="32">
         <v>2.75</v>
       </c>
-      <c r="M7" s="33">
+      <c r="M7" s="32">
         <v>3.25</v>
       </c>
-      <c r="N7" s="33">
+      <c r="N7" s="32">
         <v>3.25</v>
       </c>
-      <c r="O7" s="33">
+      <c r="O7" s="32">
         <v>3</v>
       </c>
     </row>
@@ -7182,46 +7149,46 @@
       <c r="A8" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="33">
+      <c r="B8" s="32">
         <v>3.5</v>
       </c>
-      <c r="C8" s="33">
+      <c r="C8" s="32">
         <v>3.5</v>
       </c>
-      <c r="D8" s="33">
-        <v>3</v>
-      </c>
-      <c r="E8" s="33">
+      <c r="D8" s="32">
+        <v>3</v>
+      </c>
+      <c r="E8" s="32">
         <v>3.5</v>
       </c>
-      <c r="F8" s="33">
-        <v>3</v>
-      </c>
-      <c r="G8" s="33">
+      <c r="F8" s="32">
+        <v>3</v>
+      </c>
+      <c r="G8" s="32">
         <v>3.5</v>
       </c>
-      <c r="H8" s="33">
-        <v>4</v>
-      </c>
-      <c r="I8" s="33">
+      <c r="H8" s="32">
+        <v>4</v>
+      </c>
+      <c r="I8" s="32">
         <v>2.5</v>
       </c>
-      <c r="J8" s="33">
-        <v>3</v>
-      </c>
-      <c r="K8" s="33">
+      <c r="J8" s="32">
+        <v>3</v>
+      </c>
+      <c r="K8" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="L8" s="33">
+      <c r="L8" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="M8" s="33">
-        <v>3</v>
-      </c>
-      <c r="N8" s="33">
-        <v>4</v>
-      </c>
-      <c r="O8" s="33">
+      <c r="M8" s="32">
+        <v>3</v>
+      </c>
+      <c r="N8" s="32">
+        <v>4</v>
+      </c>
+      <c r="O8" s="32">
         <v>4</v>
       </c>
     </row>
@@ -7229,46 +7196,46 @@
       <c r="A9" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>3.5</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>3.5</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>3.5</v>
       </c>
-      <c r="E9" s="33">
-        <v>4</v>
-      </c>
-      <c r="F9" s="33">
-        <v>4</v>
-      </c>
-      <c r="G9" s="33">
+      <c r="E9" s="32">
+        <v>4</v>
+      </c>
+      <c r="F9" s="32">
+        <v>4</v>
+      </c>
+      <c r="G9" s="32">
         <v>3.5</v>
       </c>
-      <c r="H9" s="33">
-        <v>4</v>
-      </c>
-      <c r="I9" s="33">
+      <c r="H9" s="32">
+        <v>4</v>
+      </c>
+      <c r="I9" s="32">
         <v>3.5</v>
       </c>
-      <c r="J9" s="33">
-        <v>4</v>
-      </c>
-      <c r="K9" s="33">
+      <c r="J9" s="32">
+        <v>4</v>
+      </c>
+      <c r="K9" s="32">
         <v>4.5</v>
       </c>
-      <c r="L9" s="33">
-        <v>4</v>
-      </c>
-      <c r="M9" s="33">
+      <c r="L9" s="32">
+        <v>4</v>
+      </c>
+      <c r="M9" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="N9" s="33">
+      <c r="N9" s="32">
         <v>4.666666666666667</v>
       </c>
-      <c r="O9" s="33">
+      <c r="O9" s="32">
         <v>4</v>
       </c>
     </row>
@@ -7276,46 +7243,46 @@
       <c r="A10" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="33">
-        <v>4</v>
-      </c>
-      <c r="C10" s="33">
-        <v>3</v>
-      </c>
-      <c r="D10" s="33">
+      <c r="B10" s="32">
+        <v>4</v>
+      </c>
+      <c r="C10" s="32">
+        <v>3</v>
+      </c>
+      <c r="D10" s="32">
         <v>3.5</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="32">
         <v>2.5</v>
       </c>
-      <c r="F10" s="33">
+      <c r="F10" s="32">
         <v>3.5</v>
       </c>
-      <c r="G10" s="33">
-        <v>3</v>
-      </c>
-      <c r="H10" s="33">
-        <v>3</v>
-      </c>
-      <c r="I10" s="33">
-        <v>3</v>
-      </c>
-      <c r="J10" s="33">
+      <c r="G10" s="32">
+        <v>3</v>
+      </c>
+      <c r="H10" s="32">
+        <v>3</v>
+      </c>
+      <c r="I10" s="32">
+        <v>3</v>
+      </c>
+      <c r="J10" s="32">
         <v>4.333333333333333</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="L10" s="33">
+      <c r="L10" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="M10" s="33">
+      <c r="M10" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="N10" s="33">
-        <v>4</v>
-      </c>
-      <c r="O10" s="33">
+      <c r="N10" s="32">
+        <v>4</v>
+      </c>
+      <c r="O10" s="32">
         <v>3</v>
       </c>
     </row>
@@ -7323,46 +7290,46 @@
       <c r="A11" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="33">
-        <v>3</v>
-      </c>
-      <c r="C11" s="33">
+      <c r="B11" s="32">
+        <v>3</v>
+      </c>
+      <c r="C11" s="32">
         <v>2.5</v>
       </c>
-      <c r="D11" s="33">
-        <v>3</v>
-      </c>
-      <c r="E11" s="33">
+      <c r="D11" s="32">
+        <v>3</v>
+      </c>
+      <c r="E11" s="32">
         <v>3.5</v>
       </c>
-      <c r="F11" s="33">
-        <v>3</v>
-      </c>
-      <c r="G11" s="33">
+      <c r="F11" s="32">
+        <v>3</v>
+      </c>
+      <c r="G11" s="32">
         <v>2.5</v>
       </c>
-      <c r="H11" s="33">
-        <v>3</v>
-      </c>
-      <c r="I11" s="33">
+      <c r="H11" s="32">
+        <v>3</v>
+      </c>
+      <c r="I11" s="32">
         <v>2.5</v>
       </c>
-      <c r="J11" s="33">
+      <c r="J11" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="K11" s="33">
-        <v>3</v>
-      </c>
-      <c r="L11" s="33">
+      <c r="K11" s="32">
+        <v>3</v>
+      </c>
+      <c r="L11" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="M11" s="33">
+      <c r="M11" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="N11" s="33">
-        <v>4</v>
-      </c>
-      <c r="O11" s="33">
+      <c r="N11" s="32">
+        <v>4</v>
+      </c>
+      <c r="O11" s="32">
         <v>3.6666666666666665</v>
       </c>
     </row>
@@ -7370,46 +7337,46 @@
       <c r="A12" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="33">
+      <c r="B12" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="C12" s="33">
-        <v>4</v>
-      </c>
-      <c r="D12" s="33">
-        <v>3</v>
-      </c>
-      <c r="E12" s="33">
-        <v>3</v>
-      </c>
-      <c r="F12" s="33">
+      <c r="C12" s="32">
+        <v>4</v>
+      </c>
+      <c r="D12" s="32">
+        <v>3</v>
+      </c>
+      <c r="E12" s="32">
+        <v>3</v>
+      </c>
+      <c r="F12" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="G12" s="33">
+      <c r="G12" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="H12" s="33">
+      <c r="H12" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="I12" s="33">
+      <c r="I12" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="J12" s="33">
+      <c r="J12" s="32">
         <v>3.75</v>
       </c>
-      <c r="K12" s="33">
-        <v>3</v>
-      </c>
-      <c r="L12" s="33">
-        <v>3</v>
-      </c>
-      <c r="M12" s="33">
-        <v>4</v>
-      </c>
-      <c r="N12" s="33">
-        <v>3</v>
-      </c>
-      <c r="O12" s="33">
+      <c r="K12" s="32">
+        <v>3</v>
+      </c>
+      <c r="L12" s="32">
+        <v>3</v>
+      </c>
+      <c r="M12" s="32">
+        <v>4</v>
+      </c>
+      <c r="N12" s="32">
+        <v>3</v>
+      </c>
+      <c r="O12" s="32">
         <v>3.5</v>
       </c>
     </row>
@@ -7417,46 +7384,46 @@
       <c r="A13" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="33">
+      <c r="B13" s="32">
         <v>1.6666666666666667</v>
       </c>
-      <c r="C13" s="33">
+      <c r="C13" s="32">
         <v>2</v>
       </c>
-      <c r="D13" s="33">
+      <c r="D13" s="32">
         <v>2.3333333333333335</v>
       </c>
-      <c r="E13" s="33">
+      <c r="E13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="F13" s="33">
+      <c r="F13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="G13" s="33">
+      <c r="G13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="H13" s="33">
+      <c r="H13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="I13" s="33">
+      <c r="I13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="J13" s="33">
-        <v>3</v>
-      </c>
-      <c r="K13" s="33">
+      <c r="J13" s="32">
+        <v>3</v>
+      </c>
+      <c r="K13" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="L13" s="33">
+      <c r="L13" s="32">
         <v>4.5</v>
       </c>
-      <c r="M13" s="33">
-        <v>4</v>
-      </c>
-      <c r="N13" s="33">
+      <c r="M13" s="32">
+        <v>4</v>
+      </c>
+      <c r="N13" s="32">
         <v>4.5</v>
       </c>
-      <c r="O13" s="33">
+      <c r="O13" s="32">
         <v>4.75</v>
       </c>
     </row>
@@ -7464,46 +7431,46 @@
       <c r="A14" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="C14" s="33">
+      <c r="C14" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="D14" s="33">
+      <c r="D14" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="E14" s="33">
+      <c r="E14" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="F14" s="33">
+      <c r="F14" s="32">
         <v>3.3333333333333335</v>
       </c>
-      <c r="G14" s="33">
+      <c r="G14" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="H14" s="33">
-        <v>3</v>
-      </c>
-      <c r="I14" s="33">
+      <c r="H14" s="32">
+        <v>3</v>
+      </c>
+      <c r="I14" s="32">
         <v>2.6666666666666665</v>
       </c>
-      <c r="J14" s="33">
+      <c r="J14" s="32">
         <v>3.75</v>
       </c>
-      <c r="K14" s="33">
+      <c r="K14" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="L14" s="33">
+      <c r="L14" s="32">
         <v>3.5</v>
       </c>
-      <c r="M14" s="33">
+      <c r="M14" s="32">
         <v>3.75</v>
       </c>
-      <c r="N14" s="33">
+      <c r="N14" s="32">
         <v>3.75</v>
       </c>
-      <c r="O14" s="33">
+      <c r="O14" s="32">
         <v>4</v>
       </c>
     </row>
@@ -7511,46 +7478,46 @@
       <c r="A15" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="33">
+      <c r="B15" s="32">
         <v>3.6666666666666665</v>
       </c>
-      <c r="C15" s="33">
-        <v>4</v>
-      </c>
-      <c r="D15" s="33">
+      <c r="C15" s="32">
+        <v>4</v>
+      </c>
+      <c r="D15" s="32">
         <v>3.5</v>
       </c>
-      <c r="E15" s="33">
+      <c r="E15" s="32">
         <v>3.25</v>
       </c>
-      <c r="F15" s="33">
+      <c r="F15" s="32">
         <v>3.75</v>
       </c>
-      <c r="G15" s="33">
-        <v>4</v>
-      </c>
-      <c r="H15" s="33">
+      <c r="G15" s="32">
+        <v>4</v>
+      </c>
+      <c r="H15" s="32">
         <v>3.5</v>
       </c>
-      <c r="I15" s="33">
+      <c r="I15" s="32">
         <v>3.25</v>
       </c>
-      <c r="J15" s="33">
+      <c r="J15" s="32">
         <v>3.5</v>
       </c>
-      <c r="K15" s="33">
-        <v>4</v>
-      </c>
-      <c r="L15" s="33">
+      <c r="K15" s="32">
+        <v>4</v>
+      </c>
+      <c r="L15" s="32">
         <v>4.25</v>
       </c>
-      <c r="M15" s="33">
+      <c r="M15" s="32">
         <v>3.75</v>
       </c>
-      <c r="N15" s="33">
+      <c r="N15" s="32">
         <v>4.5</v>
       </c>
-      <c r="O15" s="33">
+      <c r="O15" s="32">
         <v>3.75</v>
       </c>
     </row>
@@ -7558,46 +7525,46 @@
       <c r="A16" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="32">
+      <c r="B16">
         <v>3.28125</v>
       </c>
-      <c r="C16" s="32">
+      <c r="C16">
         <v>3.25</v>
       </c>
-      <c r="D16" s="32">
+      <c r="D16">
         <v>3.0909090909090908</v>
       </c>
-      <c r="E16" s="32">
+      <c r="E16">
         <v>3.393939393939394</v>
       </c>
-      <c r="F16" s="32">
+      <c r="F16">
         <v>3.4242424242424243</v>
       </c>
-      <c r="G16" s="32">
+      <c r="G16">
         <v>3.2727272727272729</v>
       </c>
-      <c r="H16" s="32">
+      <c r="H16">
         <v>3.3636363636363638</v>
       </c>
-      <c r="I16" s="32">
+      <c r="I16">
         <v>3.1212121212121211</v>
       </c>
-      <c r="J16" s="32">
+      <c r="J16">
         <v>3.65</v>
       </c>
-      <c r="K16" s="32">
+      <c r="K16">
         <v>3.5135135135135136</v>
       </c>
-      <c r="L16" s="32">
+      <c r="L16">
         <v>3.7948717948717947</v>
       </c>
-      <c r="M16" s="32">
+      <c r="M16">
         <v>3.65</v>
       </c>
-      <c r="N16" s="32">
+      <c r="N16">
         <v>4.0263157894736841</v>
       </c>
-      <c r="O16" s="32">
+      <c r="O16">
         <v>3.736842105263158</v>
       </c>
     </row>

</xml_diff>